<commit_message>
print template and iw grid acton buttn validation
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mohan\Avows\repos\RAMS\Web\RAMMS.Web.UI\wwwroot\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\source\repos\RAMMS\RAMS\Web\RAMMS.Web.UI\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -925,7 +925,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1093,6 +1093,264 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1120,275 +1378,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1429,7 +1432,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FA6B1FE-CE21-4599-9673-10530AEDAF91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7FA6B1FE-CE21-4599-9673-10530AEDAF91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1479,7 +1482,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{111F2E8A-CA78-40A1-B599-4BB69C13CA1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{111F2E8A-CA78-40A1-B599-4BB69C13CA1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1558,7 +1561,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42CB9192-A308-4EC5-89B8-8FC3409B7B5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{42CB9192-A308-4EC5-89B8-8FC3409B7B5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1984,7 +1987,7 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:K46"/>
+      <selection activeCell="B23" sqref="B23:P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,64 +2006,64 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="164" t="s">
+      <c r="D1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
-      <c r="I1" s="164"/>
-      <c r="J1" s="164"/>
-      <c r="K1" s="164"/>
-      <c r="L1" s="164"/>
-      <c r="M1" s="164"/>
-      <c r="N1" s="164"/>
-      <c r="O1" s="164"/>
-      <c r="P1" s="164"/>
-      <c r="Q1" s="165"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="78"/>
     </row>
     <row r="2" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="166" t="s">
+      <c r="D2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
-      <c r="K2" s="167"/>
-      <c r="L2" s="167"/>
-      <c r="M2" s="167"/>
-      <c r="N2" s="167"/>
-      <c r="O2" s="167"/>
-      <c r="P2" s="167"/>
-      <c r="Q2" s="168"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="81"/>
     </row>
     <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="169" t="s">
+      <c r="D3" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
-      <c r="L3" s="169"/>
-      <c r="M3" s="169"/>
-      <c r="N3" s="169"/>
-      <c r="O3" s="169"/>
-      <c r="P3" s="169"/>
-      <c r="Q3" s="170"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="83"/>
     </row>
     <row r="4" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -2102,16 +2105,16 @@
     </row>
     <row r="6" spans="1:18" ht="2.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="171"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="171"/>
-      <c r="K6" s="171"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -2121,25 +2124,25 @@
     </row>
     <row r="7" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
-      <c r="B7" s="163" t="s">
+      <c r="B7" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="157" t="s">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="157"/>
-      <c r="L7" s="159"/>
-      <c r="M7" s="159"/>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
-      <c r="P7" s="159"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.3">
@@ -2163,25 +2166,25 @@
     </row>
     <row r="9" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
-      <c r="B9" s="157" t="s">
+      <c r="B9" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="158"/>
-      <c r="F9" s="158"/>
-      <c r="G9" s="158"/>
-      <c r="H9" s="158"/>
-      <c r="I9" s="158"/>
-      <c r="J9" s="157" t="s">
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="157"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
       <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="1:18" ht="1.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2215,70 +2218,70 @@
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="160"/>
-      <c r="M11" s="160"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="85"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="161"/>
-      <c r="Q11" s="162"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="87"/>
     </row>
     <row r="12" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="144"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="144"/>
-      <c r="F12" s="144"/>
-      <c r="G12" s="144"/>
-      <c r="H12" s="144"/>
-      <c r="I12" s="144"/>
-      <c r="J12" s="144"/>
-      <c r="K12" s="144"/>
-      <c r="L12" s="144"/>
-      <c r="M12" s="144"/>
-      <c r="N12" s="144"/>
-      <c r="O12" s="144"/>
-      <c r="P12" s="144"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
       <c r="Q12" s="23"/>
     </row>
     <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="145"/>
-      <c r="C13" s="145"/>
-      <c r="D13" s="145"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="145"/>
-      <c r="G13" s="145"/>
-      <c r="H13" s="145"/>
-      <c r="I13" s="145"/>
-      <c r="J13" s="145"/>
-      <c r="K13" s="145"/>
-      <c r="L13" s="145"/>
-      <c r="M13" s="145"/>
-      <c r="N13" s="145"/>
-      <c r="O13" s="145"/>
-      <c r="P13" s="145"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
+      <c r="O13" s="90"/>
+      <c r="P13" s="90"/>
       <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:18" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="146"/>
-      <c r="C14" s="146"/>
-      <c r="D14" s="146"/>
-      <c r="E14" s="146"/>
-      <c r="F14" s="146"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="146"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="146"/>
-      <c r="K14" s="146"/>
-      <c r="L14" s="146"/>
-      <c r="M14" s="146"/>
-      <c r="N14" s="146"/>
-      <c r="O14" s="146"/>
-      <c r="P14" s="146"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="91"/>
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2305,67 +2308,67 @@
     </row>
     <row r="16" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="147"/>
-      <c r="D16" s="148"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
-      <c r="G16" s="148"/>
-      <c r="H16" s="147" t="s">
+      <c r="C16" s="92"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="147"/>
-      <c r="J16" s="147"/>
-      <c r="K16" s="147"/>
-      <c r="L16" s="149"/>
-      <c r="M16" s="149"/>
-      <c r="N16" s="149"/>
-      <c r="O16" s="149"/>
-      <c r="P16" s="149"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="94"/>
+      <c r="P16" s="94"/>
       <c r="Q16" s="30"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="150"/>
-      <c r="D17" s="151"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="151"/>
-      <c r="H17" s="151"/>
-      <c r="I17" s="151"/>
-      <c r="J17" s="151"/>
-      <c r="K17" s="151"/>
-      <c r="L17" s="153" t="s">
+      <c r="C17" s="95"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="154"/>
-      <c r="N17" s="154"/>
-      <c r="O17" s="154"/>
-      <c r="P17" s="154"/>
+      <c r="M17" s="99"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="99"/>
+      <c r="P17" s="99"/>
       <c r="Q17" s="32"/>
     </row>
     <row r="18" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="150"/>
-      <c r="C18" s="150"/>
-      <c r="D18" s="152"/>
-      <c r="E18" s="152"/>
-      <c r="F18" s="152"/>
-      <c r="G18" s="152"/>
-      <c r="H18" s="152"/>
-      <c r="I18" s="152"/>
-      <c r="J18" s="152"/>
-      <c r="K18" s="152"/>
-      <c r="L18" s="155"/>
-      <c r="M18" s="156"/>
-      <c r="N18" s="156"/>
-      <c r="O18" s="156"/>
-      <c r="P18" s="156"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="97"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="101"/>
+      <c r="N18" s="101"/>
+      <c r="O18" s="101"/>
+      <c r="P18" s="101"/>
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:18" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2408,159 +2411,159 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="136"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="136"/>
-      <c r="H21" s="136"/>
-      <c r="I21" s="136"/>
-      <c r="J21" s="136"/>
-      <c r="K21" s="136"/>
-      <c r="L21" s="136"/>
-      <c r="M21" s="136"/>
-      <c r="N21" s="136"/>
-      <c r="O21" s="136"/>
-      <c r="P21" s="136"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="88"/>
+      <c r="P21" s="88"/>
       <c r="Q21" s="27"/>
       <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="137" t="s">
+      <c r="A22" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="138"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="138"/>
-      <c r="I22" s="138"/>
-      <c r="J22" s="138"/>
-      <c r="K22" s="138"/>
-      <c r="L22" s="138"/>
-      <c r="M22" s="138"/>
-      <c r="N22" s="138"/>
-      <c r="O22" s="138"/>
-      <c r="P22" s="138"/>
-      <c r="Q22" s="139"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="103"/>
+      <c r="I22" s="103"/>
+      <c r="J22" s="103"/>
+      <c r="K22" s="103"/>
+      <c r="L22" s="103"/>
+      <c r="M22" s="103"/>
+      <c r="N22" s="103"/>
+      <c r="O22" s="103"/>
+      <c r="P22" s="103"/>
+      <c r="Q22" s="104"/>
     </row>
     <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
-      <c r="B23" s="140"/>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="140"/>
-      <c r="J23" s="140"/>
-      <c r="K23" s="140"/>
-      <c r="L23" s="140"/>
-      <c r="M23" s="140"/>
-      <c r="N23" s="140"/>
-      <c r="O23" s="140"/>
-      <c r="P23" s="140"/>
+      <c r="B23" s="172"/>
+      <c r="C23" s="172"/>
+      <c r="D23" s="172"/>
+      <c r="E23" s="172"/>
+      <c r="F23" s="172"/>
+      <c r="G23" s="172"/>
+      <c r="H23" s="172"/>
+      <c r="I23" s="172"/>
+      <c r="J23" s="172"/>
+      <c r="K23" s="172"/>
+      <c r="L23" s="172"/>
+      <c r="M23" s="172"/>
+      <c r="N23" s="172"/>
+      <c r="O23" s="172"/>
+      <c r="P23" s="172"/>
       <c r="Q23" s="16"/>
     </row>
     <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="140"/>
-      <c r="C24" s="140"/>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="140"/>
-      <c r="H24" s="140"/>
-      <c r="I24" s="140"/>
-      <c r="J24" s="140"/>
-      <c r="K24" s="140"/>
-      <c r="L24" s="140"/>
-      <c r="M24" s="140"/>
-      <c r="N24" s="140"/>
-      <c r="O24" s="140"/>
-      <c r="P24" s="140"/>
+      <c r="B24" s="172"/>
+      <c r="C24" s="172"/>
+      <c r="D24" s="172"/>
+      <c r="E24" s="172"/>
+      <c r="F24" s="172"/>
+      <c r="G24" s="172"/>
+      <c r="H24" s="172"/>
+      <c r="I24" s="172"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="172"/>
+      <c r="L24" s="172"/>
+      <c r="M24" s="172"/>
+      <c r="N24" s="172"/>
+      <c r="O24" s="172"/>
+      <c r="P24" s="172"/>
       <c r="Q24" s="16"/>
     </row>
     <row r="25" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
-      <c r="B25" s="140"/>
-      <c r="C25" s="140"/>
-      <c r="D25" s="140"/>
-      <c r="E25" s="140"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="140"/>
-      <c r="I25" s="140"/>
-      <c r="J25" s="140"/>
-      <c r="K25" s="140"/>
-      <c r="L25" s="140"/>
-      <c r="M25" s="140"/>
-      <c r="N25" s="140"/>
-      <c r="O25" s="140"/>
-      <c r="P25" s="140"/>
+      <c r="B25" s="172"/>
+      <c r="C25" s="172"/>
+      <c r="D25" s="172"/>
+      <c r="E25" s="172"/>
+      <c r="F25" s="172"/>
+      <c r="G25" s="172"/>
+      <c r="H25" s="172"/>
+      <c r="I25" s="172"/>
+      <c r="J25" s="172"/>
+      <c r="K25" s="172"/>
+      <c r="L25" s="172"/>
+      <c r="M25" s="172"/>
+      <c r="N25" s="172"/>
+      <c r="O25" s="172"/>
+      <c r="P25" s="172"/>
       <c r="Q25" s="16"/>
     </row>
     <row r="26" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
-      <c r="B26" s="140"/>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="140"/>
-      <c r="K26" s="140"/>
-      <c r="L26" s="140"/>
-      <c r="M26" s="140"/>
-      <c r="N26" s="140"/>
-      <c r="O26" s="140"/>
-      <c r="P26" s="140"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="172"/>
+      <c r="D26" s="172"/>
+      <c r="E26" s="172"/>
+      <c r="F26" s="172"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="172"/>
+      <c r="I26" s="172"/>
+      <c r="J26" s="172"/>
+      <c r="K26" s="172"/>
+      <c r="L26" s="172"/>
+      <c r="M26" s="172"/>
+      <c r="N26" s="172"/>
+      <c r="O26" s="172"/>
+      <c r="P26" s="172"/>
       <c r="Q26" s="16"/>
     </row>
     <row r="27" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
-      <c r="B27" s="140"/>
-      <c r="C27" s="140"/>
-      <c r="D27" s="140"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="140"/>
-      <c r="G27" s="140"/>
-      <c r="H27" s="140"/>
-      <c r="I27" s="140"/>
-      <c r="J27" s="140"/>
-      <c r="K27" s="140"/>
-      <c r="L27" s="140"/>
-      <c r="M27" s="140"/>
-      <c r="N27" s="140"/>
-      <c r="O27" s="140"/>
-      <c r="P27" s="140"/>
+      <c r="B27" s="172"/>
+      <c r="C27" s="172"/>
+      <c r="D27" s="172"/>
+      <c r="E27" s="172"/>
+      <c r="F27" s="172"/>
+      <c r="G27" s="172"/>
+      <c r="H27" s="172"/>
+      <c r="I27" s="172"/>
+      <c r="J27" s="172"/>
+      <c r="K27" s="172"/>
+      <c r="L27" s="172"/>
+      <c r="M27" s="172"/>
+      <c r="N27" s="172"/>
+      <c r="O27" s="172"/>
+      <c r="P27" s="172"/>
       <c r="Q27" s="16"/>
     </row>
     <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
-      <c r="B28" s="140"/>
-      <c r="C28" s="140"/>
-      <c r="D28" s="140"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="140"/>
-      <c r="G28" s="140"/>
-      <c r="H28" s="140"/>
-      <c r="I28" s="140"/>
-      <c r="J28" s="140"/>
-      <c r="K28" s="140"/>
-      <c r="L28" s="140"/>
-      <c r="M28" s="140"/>
-      <c r="N28" s="140"/>
-      <c r="O28" s="140"/>
-      <c r="P28" s="140"/>
+      <c r="B28" s="171"/>
+      <c r="C28" s="171"/>
+      <c r="D28" s="171"/>
+      <c r="E28" s="171"/>
+      <c r="F28" s="171"/>
+      <c r="G28" s="171"/>
+      <c r="H28" s="171"/>
+      <c r="I28" s="171"/>
+      <c r="J28" s="171"/>
+      <c r="K28" s="171"/>
+      <c r="L28" s="171"/>
+      <c r="M28" s="171"/>
+      <c r="N28" s="171"/>
+      <c r="O28" s="171"/>
+      <c r="P28" s="171"/>
       <c r="Q28" s="16"/>
     </row>
     <row r="29" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
@@ -2584,386 +2587,386 @@
     </row>
     <row r="30" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
-      <c r="B30" s="141" t="s">
+      <c r="B30" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="141"/>
-      <c r="D30" s="141"/>
+      <c r="C30" s="105"/>
+      <c r="D30" s="105"/>
       <c r="E30" s="43"/>
-      <c r="F30" s="141" t="s">
+      <c r="F30" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="142"/>
-      <c r="H30" s="143" t="s">
+      <c r="G30" s="106"/>
+      <c r="H30" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="141"/>
-      <c r="J30" s="141"/>
-      <c r="K30" s="141"/>
-      <c r="L30" s="141"/>
-      <c r="M30" s="141"/>
+      <c r="I30" s="105"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="105"/>
+      <c r="L30" s="105"/>
+      <c r="M30" s="105"/>
       <c r="N30" s="44"/>
-      <c r="O30" s="141" t="s">
+      <c r="O30" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="P30" s="141"/>
+      <c r="P30" s="105"/>
       <c r="Q30" s="45"/>
     </row>
     <row r="31" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46"/>
-      <c r="B32" s="136" t="s">
+      <c r="B32" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="136"/>
-      <c r="D32" s="136"/>
-      <c r="E32" s="136"/>
-      <c r="F32" s="136"/>
-      <c r="G32" s="136"/>
-      <c r="H32" s="136"/>
-      <c r="I32" s="136"/>
-      <c r="J32" s="136"/>
-      <c r="K32" s="136"/>
-      <c r="L32" s="136"/>
-      <c r="M32" s="136"/>
-      <c r="N32" s="136"/>
-      <c r="O32" s="136"/>
-      <c r="P32" s="136"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="88"/>
+      <c r="H32" s="88"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="88"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="88"/>
+      <c r="M32" s="88"/>
+      <c r="N32" s="88"/>
+      <c r="O32" s="88"/>
+      <c r="P32" s="88"/>
       <c r="Q32" s="47"/>
     </row>
     <row r="33" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48"/>
-      <c r="B33" s="132" t="s">
+      <c r="B33" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="132"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="132"/>
-      <c r="F33" s="132"/>
-      <c r="G33" s="132"/>
-      <c r="H33" s="132"/>
-      <c r="I33" s="132"/>
-      <c r="J33" s="132"/>
-      <c r="K33" s="132"/>
-      <c r="L33" s="133"/>
-      <c r="M33" s="134"/>
-      <c r="N33" s="135"/>
-      <c r="O33" s="135"/>
-      <c r="P33" s="135"/>
+      <c r="C33" s="108"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="108"/>
+      <c r="G33" s="108"/>
+      <c r="H33" s="108"/>
+      <c r="I33" s="108"/>
+      <c r="J33" s="108"/>
+      <c r="K33" s="108"/>
+      <c r="L33" s="109"/>
+      <c r="M33" s="110"/>
+      <c r="N33" s="111"/>
+      <c r="O33" s="111"/>
+      <c r="P33" s="111"/>
       <c r="Q33" s="49"/>
     </row>
     <row r="34" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
-      <c r="B34" s="128" t="s">
+      <c r="B34" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="128"/>
-      <c r="D34" s="128"/>
-      <c r="E34" s="128"/>
-      <c r="F34" s="128"/>
-      <c r="G34" s="128"/>
-      <c r="H34" s="128"/>
-      <c r="I34" s="128"/>
-      <c r="J34" s="128"/>
-      <c r="K34" s="128"/>
-      <c r="L34" s="129"/>
-      <c r="M34" s="130"/>
-      <c r="N34" s="131"/>
-      <c r="O34" s="131"/>
-      <c r="P34" s="131"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="114"/>
+      <c r="N34" s="115"/>
+      <c r="O34" s="115"/>
+      <c r="P34" s="115"/>
       <c r="Q34" s="51"/>
     </row>
     <row r="35" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
-      <c r="B35" s="128" t="s">
+      <c r="B35" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="128"/>
-      <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="128"/>
-      <c r="G35" s="128"/>
-      <c r="H35" s="128"/>
-      <c r="I35" s="128"/>
-      <c r="J35" s="128"/>
-      <c r="K35" s="128"/>
-      <c r="L35" s="129"/>
-      <c r="M35" s="130"/>
-      <c r="N35" s="131"/>
-      <c r="O35" s="131"/>
-      <c r="P35" s="131"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="112"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="112"/>
+      <c r="K35" s="112"/>
+      <c r="L35" s="113"/>
+      <c r="M35" s="114"/>
+      <c r="N35" s="115"/>
+      <c r="O35" s="115"/>
+      <c r="P35" s="115"/>
       <c r="Q35" s="51"/>
     </row>
     <row r="36" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
-      <c r="B36" s="128" t="s">
+      <c r="B36" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="128"/>
-      <c r="D36" s="128"/>
-      <c r="E36" s="128"/>
-      <c r="F36" s="128"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="128"/>
-      <c r="I36" s="128"/>
-      <c r="J36" s="128"/>
-      <c r="K36" s="128"/>
-      <c r="L36" s="129"/>
-      <c r="M36" s="130"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="131"/>
-      <c r="P36" s="131"/>
+      <c r="C36" s="112"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="112"/>
+      <c r="G36" s="112"/>
+      <c r="H36" s="112"/>
+      <c r="I36" s="112"/>
+      <c r="J36" s="112"/>
+      <c r="K36" s="112"/>
+      <c r="L36" s="113"/>
+      <c r="M36" s="114"/>
+      <c r="N36" s="115"/>
+      <c r="O36" s="115"/>
+      <c r="P36" s="115"/>
       <c r="Q36" s="51"/>
     </row>
     <row r="37" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
-      <c r="B37" s="128" t="s">
+      <c r="B37" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="128"/>
-      <c r="D37" s="128"/>
-      <c r="E37" s="128"/>
-      <c r="F37" s="128"/>
-      <c r="G37" s="128"/>
-      <c r="H37" s="128"/>
-      <c r="I37" s="128"/>
-      <c r="J37" s="128"/>
-      <c r="K37" s="128"/>
-      <c r="L37" s="129"/>
-      <c r="M37" s="130"/>
-      <c r="N37" s="131"/>
-      <c r="O37" s="131"/>
-      <c r="P37" s="131"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="112"/>
+      <c r="G37" s="112"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
+      <c r="K37" s="112"/>
+      <c r="L37" s="113"/>
+      <c r="M37" s="114"/>
+      <c r="N37" s="115"/>
+      <c r="O37" s="115"/>
+      <c r="P37" s="115"/>
       <c r="Q37" s="51"/>
     </row>
     <row r="38" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
-      <c r="B38" s="128" t="s">
+      <c r="B38" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="128"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="128"/>
-      <c r="F38" s="128"/>
-      <c r="G38" s="128"/>
-      <c r="H38" s="128"/>
-      <c r="I38" s="128"/>
-      <c r="J38" s="128"/>
-      <c r="K38" s="128"/>
-      <c r="L38" s="129"/>
-      <c r="M38" s="130"/>
-      <c r="N38" s="131"/>
-      <c r="O38" s="131"/>
-      <c r="P38" s="131"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="112"/>
+      <c r="H38" s="112"/>
+      <c r="I38" s="112"/>
+      <c r="J38" s="112"/>
+      <c r="K38" s="112"/>
+      <c r="L38" s="113"/>
+      <c r="M38" s="114"/>
+      <c r="N38" s="115"/>
+      <c r="O38" s="115"/>
+      <c r="P38" s="115"/>
       <c r="Q38" s="51"/>
     </row>
     <row r="39" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
-      <c r="B39" s="101" t="s">
+      <c r="B39" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101"/>
-      <c r="G39" s="101"/>
-      <c r="H39" s="101"/>
-      <c r="I39" s="101"/>
-      <c r="J39" s="101"/>
-      <c r="K39" s="101"/>
-      <c r="L39" s="102"/>
-      <c r="M39" s="103"/>
-      <c r="N39" s="104"/>
-      <c r="O39" s="104"/>
-      <c r="P39" s="104"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
+      <c r="G39" s="116"/>
+      <c r="H39" s="116"/>
+      <c r="I39" s="116"/>
+      <c r="J39" s="116"/>
+      <c r="K39" s="116"/>
+      <c r="L39" s="117"/>
+      <c r="M39" s="118"/>
+      <c r="N39" s="119"/>
+      <c r="O39" s="119"/>
+      <c r="P39" s="119"/>
       <c r="Q39" s="53"/>
     </row>
     <row r="40" spans="1:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:17" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="54"/>
-      <c r="B41" s="105" t="s">
+      <c r="B41" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="105"/>
-      <c r="D41" s="107" t="s">
+      <c r="C41" s="120"/>
+      <c r="D41" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="108"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="113" t="s">
+      <c r="E41" s="123"/>
+      <c r="F41" s="124"/>
+      <c r="G41" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
-      <c r="J41" s="114"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="117" t="s">
+      <c r="H41" s="129"/>
+      <c r="I41" s="129"/>
+      <c r="J41" s="129"/>
+      <c r="K41" s="129"/>
+      <c r="L41" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="M41" s="118"/>
-      <c r="N41" s="118"/>
-      <c r="O41" s="118"/>
-      <c r="P41" s="118"/>
+      <c r="M41" s="133"/>
+      <c r="N41" s="133"/>
+      <c r="O41" s="133"/>
+      <c r="P41" s="133"/>
       <c r="Q41" s="55"/>
     </row>
     <row r="42" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
-      <c r="B42" s="106"/>
-      <c r="C42" s="106"/>
-      <c r="D42" s="110"/>
-      <c r="E42" s="111"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="115"/>
-      <c r="H42" s="116"/>
-      <c r="I42" s="116"/>
-      <c r="J42" s="116"/>
-      <c r="K42" s="116"/>
-      <c r="L42" s="119"/>
-      <c r="M42" s="120"/>
-      <c r="N42" s="120"/>
-      <c r="O42" s="120"/>
-      <c r="P42" s="120"/>
+      <c r="B42" s="121"/>
+      <c r="C42" s="121"/>
+      <c r="D42" s="125"/>
+      <c r="E42" s="126"/>
+      <c r="F42" s="127"/>
+      <c r="G42" s="130"/>
+      <c r="H42" s="131"/>
+      <c r="I42" s="131"/>
+      <c r="J42" s="131"/>
+      <c r="K42" s="131"/>
+      <c r="L42" s="134"/>
+      <c r="M42" s="135"/>
+      <c r="N42" s="135"/>
+      <c r="O42" s="135"/>
+      <c r="P42" s="135"/>
       <c r="Q42" s="57"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
-      <c r="B43" s="106"/>
-      <c r="C43" s="106"/>
-      <c r="D43" s="110"/>
-      <c r="E43" s="111"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="115"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="116"/>
-      <c r="J43" s="116"/>
-      <c r="K43" s="116"/>
-      <c r="L43" s="119"/>
-      <c r="M43" s="120"/>
-      <c r="N43" s="120"/>
-      <c r="O43" s="120"/>
-      <c r="P43" s="120"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="126"/>
+      <c r="F43" s="127"/>
+      <c r="G43" s="130"/>
+      <c r="H43" s="131"/>
+      <c r="I43" s="131"/>
+      <c r="J43" s="131"/>
+      <c r="K43" s="131"/>
+      <c r="L43" s="134"/>
+      <c r="M43" s="135"/>
+      <c r="N43" s="135"/>
+      <c r="O43" s="135"/>
+      <c r="P43" s="135"/>
       <c r="Q43" s="57"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="56"/>
-      <c r="B44" s="106"/>
-      <c r="C44" s="106"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="122"/>
-      <c r="F44" s="123"/>
-      <c r="G44" s="124"/>
-      <c r="H44" s="125"/>
-      <c r="I44" s="125"/>
-      <c r="J44" s="125"/>
-      <c r="K44" s="125"/>
-      <c r="L44" s="126"/>
-      <c r="M44" s="127"/>
-      <c r="N44" s="127"/>
-      <c r="O44" s="127"/>
-      <c r="P44" s="127"/>
+      <c r="B44" s="121"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="138"/>
+      <c r="G44" s="139"/>
+      <c r="H44" s="140"/>
+      <c r="I44" s="140"/>
+      <c r="J44" s="140"/>
+      <c r="K44" s="140"/>
+      <c r="L44" s="141"/>
+      <c r="M44" s="142"/>
+      <c r="N44" s="142"/>
+      <c r="O44" s="142"/>
+      <c r="P44" s="142"/>
       <c r="Q44" s="57"/>
     </row>
     <row r="45" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56"/>
-      <c r="B45" s="106"/>
-      <c r="C45" s="106"/>
-      <c r="D45" s="121"/>
-      <c r="E45" s="122"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="125"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="125"/>
-      <c r="K45" s="125"/>
-      <c r="L45" s="126"/>
-      <c r="M45" s="127"/>
-      <c r="N45" s="127"/>
-      <c r="O45" s="127"/>
-      <c r="P45" s="127"/>
+      <c r="B45" s="121"/>
+      <c r="C45" s="121"/>
+      <c r="D45" s="136"/>
+      <c r="E45" s="137"/>
+      <c r="F45" s="138"/>
+      <c r="G45" s="139"/>
+      <c r="H45" s="140"/>
+      <c r="I45" s="140"/>
+      <c r="J45" s="140"/>
+      <c r="K45" s="140"/>
+      <c r="L45" s="141"/>
+      <c r="M45" s="142"/>
+      <c r="N45" s="142"/>
+      <c r="O45" s="142"/>
+      <c r="P45" s="142"/>
       <c r="Q45" s="57"/>
     </row>
     <row r="46" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="58"/>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="93"/>
-      <c r="G46" s="94"/>
-      <c r="H46" s="95"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="95"/>
-      <c r="K46" s="95"/>
-      <c r="L46" s="96"/>
-      <c r="M46" s="97"/>
-      <c r="N46" s="97"/>
-      <c r="O46" s="97"/>
-      <c r="P46" s="97"/>
+      <c r="C46" s="143"/>
+      <c r="D46" s="144"/>
+      <c r="E46" s="145"/>
+      <c r="F46" s="146"/>
+      <c r="G46" s="147"/>
+      <c r="H46" s="148"/>
+      <c r="I46" s="148"/>
+      <c r="J46" s="148"/>
+      <c r="K46" s="148"/>
+      <c r="L46" s="149"/>
+      <c r="M46" s="150"/>
+      <c r="N46" s="150"/>
+      <c r="O46" s="150"/>
+      <c r="P46" s="150"/>
       <c r="Q46" s="59"/>
     </row>
     <row r="47" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
-      <c r="B47" s="82" t="s">
+      <c r="B47" s="151" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="82"/>
-      <c r="D47" s="83"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="87"/>
-      <c r="I47" s="87"/>
-      <c r="J47" s="87"/>
-      <c r="K47" s="87"/>
-      <c r="L47" s="99"/>
-      <c r="M47" s="100"/>
-      <c r="N47" s="100"/>
-      <c r="O47" s="100"/>
-      <c r="P47" s="100"/>
+      <c r="C47" s="151"/>
+      <c r="D47" s="152"/>
+      <c r="E47" s="153"/>
+      <c r="F47" s="154"/>
+      <c r="G47" s="155"/>
+      <c r="H47" s="156"/>
+      <c r="I47" s="156"/>
+      <c r="J47" s="156"/>
+      <c r="K47" s="156"/>
+      <c r="L47" s="157"/>
+      <c r="M47" s="158"/>
+      <c r="N47" s="158"/>
+      <c r="O47" s="158"/>
+      <c r="P47" s="158"/>
       <c r="Q47" s="62"/>
     </row>
     <row r="48" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="63"/>
-      <c r="B48" s="74" t="s">
+      <c r="B48" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="74"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="80"/>
-      <c r="M48" s="81"/>
-      <c r="N48" s="81"/>
-      <c r="O48" s="81"/>
-      <c r="P48" s="81"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="161"/>
+      <c r="E48" s="162"/>
+      <c r="F48" s="163"/>
+      <c r="G48" s="164"/>
+      <c r="H48" s="165"/>
+      <c r="I48" s="165"/>
+      <c r="J48" s="165"/>
+      <c r="K48" s="165"/>
+      <c r="L48" s="166"/>
+      <c r="M48" s="167"/>
+      <c r="N48" s="167"/>
+      <c r="O48" s="167"/>
+      <c r="P48" s="167"/>
       <c r="Q48" s="64"/>
     </row>
     <row r="49" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="61"/>
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="82"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="84"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="86"/>
-      <c r="H49" s="87"/>
-      <c r="I49" s="87"/>
-      <c r="J49" s="87"/>
-      <c r="K49" s="87"/>
-      <c r="L49" s="88"/>
-      <c r="M49" s="89"/>
-      <c r="N49" s="89"/>
-      <c r="O49" s="89"/>
-      <c r="P49" s="89"/>
+      <c r="C49" s="151"/>
+      <c r="D49" s="152"/>
+      <c r="E49" s="153"/>
+      <c r="F49" s="154"/>
+      <c r="G49" s="168"/>
+      <c r="H49" s="156"/>
+      <c r="I49" s="156"/>
+      <c r="J49" s="156"/>
+      <c r="K49" s="156"/>
+      <c r="L49" s="169"/>
+      <c r="M49" s="170"/>
+      <c r="N49" s="170"/>
+      <c r="O49" s="170"/>
+      <c r="P49" s="170"/>
       <c r="Q49" s="62"/>
     </row>
     <row r="50" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2989,42 +2992,72 @@
     </row>
     <row r="51" spans="1:17" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="71"/>
-      <c r="B51" s="73" t="s">
+      <c r="B51" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="73"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="73"/>
-      <c r="I51" s="73"/>
-      <c r="J51" s="73"/>
-      <c r="K51" s="73"/>
-      <c r="L51" s="73"/>
-      <c r="M51" s="73"/>
-      <c r="N51" s="73"/>
-      <c r="O51" s="73"/>
-      <c r="P51" s="73"/>
+      <c r="C51" s="159"/>
+      <c r="D51" s="159"/>
+      <c r="E51" s="159"/>
+      <c r="F51" s="159"/>
+      <c r="G51" s="159"/>
+      <c r="H51" s="159"/>
+      <c r="I51" s="159"/>
+      <c r="J51" s="159"/>
+      <c r="K51" s="159"/>
+      <c r="L51" s="159"/>
+      <c r="M51" s="159"/>
+      <c r="N51" s="159"/>
+      <c r="O51" s="159"/>
+      <c r="P51" s="159"/>
       <c r="Q51" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="D1:Q1"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D3:Q3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="P11:Q11"/>
+  <mergeCells count="72">
+    <mergeCell ref="B51:P51"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="G48:K48"/>
+    <mergeCell ref="L48:P48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="G49:K49"/>
+    <mergeCell ref="L49:P49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="L46:P46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="L47:P47"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="D41:F43"/>
+    <mergeCell ref="G41:K43"/>
+    <mergeCell ref="L41:P43"/>
+    <mergeCell ref="D44:F45"/>
+    <mergeCell ref="G44:K45"/>
+    <mergeCell ref="L44:P45"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="A22:Q22"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="B23:P28"/>
     <mergeCell ref="B21:P21"/>
     <mergeCell ref="B12:P13"/>
     <mergeCell ref="B14:P14"/>
@@ -3037,56 +3070,21 @@
     <mergeCell ref="L17:P17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="L18:P18"/>
-    <mergeCell ref="B32:P32"/>
-    <mergeCell ref="A22:Q22"/>
-    <mergeCell ref="B23:P23"/>
-    <mergeCell ref="B24:P24"/>
-    <mergeCell ref="B25:P25"/>
-    <mergeCell ref="B26:P26"/>
-    <mergeCell ref="B27:P27"/>
-    <mergeCell ref="B28:P28"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="M37:P37"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D41:F43"/>
-    <mergeCell ref="G41:K43"/>
-    <mergeCell ref="L41:P43"/>
-    <mergeCell ref="D44:F45"/>
-    <mergeCell ref="G44:K45"/>
-    <mergeCell ref="L44:P45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="L46:P46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="L47:P47"/>
-    <mergeCell ref="B51:P51"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="L48:P48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="G49:K49"/>
-    <mergeCell ref="L49:P49"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="D1:Q1"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D3:Q3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
@@ -3098,12 +3096,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3324,15 +3319,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3357,18 +3364,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
w1 and w2 and lading pages
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
@@ -1093,18 +1093,276 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1129,269 +1387,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1432,7 +1432,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7FA6B1FE-CE21-4599-9673-10530AEDAF91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FA6B1FE-CE21-4599-9673-10530AEDAF91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1482,7 +1482,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{111F2E8A-CA78-40A1-B599-4BB69C13CA1C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{111F2E8A-CA78-40A1-B599-4BB69C13CA1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1561,7 +1561,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{42CB9192-A308-4EC5-89B8-8FC3409B7B5B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42CB9192-A308-4EC5-89B8-8FC3409B7B5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1987,7 +1987,7 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:P28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,64 +2006,64 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="163" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="78"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="164"/>
     </row>
     <row r="2" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="81"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="166"/>
+      <c r="Q2" s="167"/>
     </row>
     <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="83"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="168"/>
+      <c r="M3" s="168"/>
+      <c r="N3" s="168"/>
+      <c r="O3" s="168"/>
+      <c r="P3" s="168"/>
+      <c r="Q3" s="169"/>
     </row>
     <row r="4" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -2105,16 +2105,16 @@
     </row>
     <row r="6" spans="1:18" ht="2.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
+      <c r="B6" s="170"/>
+      <c r="C6" s="170"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="J6" s="170"/>
+      <c r="K6" s="170"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -2124,25 +2124,25 @@
     </row>
     <row r="7" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75" t="s">
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="157"/>
+      <c r="F7" s="157"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="75"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
+      <c r="K7" s="156"/>
+      <c r="L7" s="158"/>
+      <c r="M7" s="158"/>
+      <c r="N7" s="158"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="158"/>
       <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.3">
@@ -2166,25 +2166,25 @@
     </row>
     <row r="9" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="156" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="75" t="s">
+      <c r="C9" s="156"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="157"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="75"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
+      <c r="K9" s="156"/>
+      <c r="L9" s="158"/>
+      <c r="M9" s="158"/>
+      <c r="N9" s="158"/>
+      <c r="O9" s="158"/>
+      <c r="P9" s="158"/>
       <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="1:18" ht="1.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2218,70 +2218,70 @@
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="85"/>
+      <c r="L11" s="159"/>
+      <c r="M11" s="159"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="87"/>
+      <c r="P11" s="160"/>
+      <c r="Q11" s="161"/>
     </row>
     <row r="12" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="143"/>
+      <c r="F12" s="143"/>
+      <c r="G12" s="143"/>
+      <c r="H12" s="143"/>
+      <c r="I12" s="143"/>
+      <c r="J12" s="143"/>
+      <c r="K12" s="143"/>
+      <c r="L12" s="143"/>
+      <c r="M12" s="143"/>
+      <c r="N12" s="143"/>
+      <c r="O12" s="143"/>
+      <c r="P12" s="143"/>
       <c r="Q12" s="23"/>
     </row>
     <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
+      <c r="G13" s="144"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
+      <c r="J13" s="144"/>
+      <c r="K13" s="144"/>
+      <c r="L13" s="144"/>
+      <c r="M13" s="144"/>
+      <c r="N13" s="144"/>
+      <c r="O13" s="144"/>
+      <c r="P13" s="144"/>
       <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:18" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-      <c r="N14" s="91"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="91"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="145"/>
+      <c r="E14" s="145"/>
+      <c r="F14" s="145"/>
+      <c r="G14" s="145"/>
+      <c r="H14" s="145"/>
+      <c r="I14" s="145"/>
+      <c r="J14" s="145"/>
+      <c r="K14" s="145"/>
+      <c r="L14" s="145"/>
+      <c r="M14" s="145"/>
+      <c r="N14" s="145"/>
+      <c r="O14" s="145"/>
+      <c r="P14" s="145"/>
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2308,67 +2308,67 @@
     </row>
     <row r="16" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="92" t="s">
+      <c r="C16" s="146"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="147"/>
+      <c r="F16" s="147"/>
+      <c r="G16" s="147"/>
+      <c r="H16" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="94"/>
-      <c r="M16" s="94"/>
-      <c r="N16" s="94"/>
-      <c r="O16" s="94"/>
-      <c r="P16" s="94"/>
+      <c r="I16" s="146"/>
+      <c r="J16" s="146"/>
+      <c r="K16" s="146"/>
+      <c r="L16" s="148"/>
+      <c r="M16" s="148"/>
+      <c r="N16" s="148"/>
+      <c r="O16" s="148"/>
+      <c r="P16" s="148"/>
       <c r="Q16" s="30"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="98" t="s">
+      <c r="C17" s="149"/>
+      <c r="D17" s="150"/>
+      <c r="E17" s="150"/>
+      <c r="F17" s="150"/>
+      <c r="G17" s="150"/>
+      <c r="H17" s="150"/>
+      <c r="I17" s="150"/>
+      <c r="J17" s="150"/>
+      <c r="K17" s="150"/>
+      <c r="L17" s="152" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="99"/>
-      <c r="N17" s="99"/>
-      <c r="O17" s="99"/>
-      <c r="P17" s="99"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="153"/>
+      <c r="O17" s="153"/>
+      <c r="P17" s="153"/>
       <c r="Q17" s="32"/>
     </row>
     <row r="18" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="97"/>
-      <c r="G18" s="97"/>
-      <c r="H18" s="97"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="97"/>
-      <c r="K18" s="97"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="101"/>
-      <c r="N18" s="101"/>
-      <c r="O18" s="101"/>
-      <c r="P18" s="101"/>
+      <c r="B18" s="149"/>
+      <c r="C18" s="149"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="151"/>
+      <c r="J18" s="151"/>
+      <c r="K18" s="151"/>
+      <c r="L18" s="154"/>
+      <c r="M18" s="155"/>
+      <c r="N18" s="155"/>
+      <c r="O18" s="155"/>
+      <c r="P18" s="155"/>
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:18" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2411,159 +2411,159 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
-      <c r="B21" s="88" t="s">
+      <c r="B21" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="88"/>
-      <c r="N21" s="88"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="88"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="136"/>
+      <c r="G21" s="136"/>
+      <c r="H21" s="136"/>
+      <c r="I21" s="136"/>
+      <c r="J21" s="136"/>
+      <c r="K21" s="136"/>
+      <c r="L21" s="136"/>
+      <c r="M21" s="136"/>
+      <c r="N21" s="136"/>
+      <c r="O21" s="136"/>
+      <c r="P21" s="136"/>
       <c r="Q21" s="27"/>
       <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="102" t="s">
+      <c r="A22" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="103"/>
-      <c r="H22" s="103"/>
-      <c r="I22" s="103"/>
-      <c r="J22" s="103"/>
-      <c r="K22" s="103"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
-      <c r="N22" s="103"/>
-      <c r="O22" s="103"/>
-      <c r="P22" s="103"/>
-      <c r="Q22" s="104"/>
+      <c r="B22" s="138"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="138"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="138"/>
+      <c r="N22" s="138"/>
+      <c r="O22" s="138"/>
+      <c r="P22" s="138"/>
+      <c r="Q22" s="139"/>
     </row>
     <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
-      <c r="B23" s="172"/>
-      <c r="C23" s="172"/>
-      <c r="D23" s="172"/>
-      <c r="E23" s="172"/>
-      <c r="F23" s="172"/>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172"/>
-      <c r="J23" s="172"/>
-      <c r="K23" s="172"/>
-      <c r="L23" s="172"/>
-      <c r="M23" s="172"/>
-      <c r="N23" s="172"/>
-      <c r="O23" s="172"/>
-      <c r="P23" s="172"/>
+      <c r="B23" s="171"/>
+      <c r="C23" s="171"/>
+      <c r="D23" s="171"/>
+      <c r="E23" s="171"/>
+      <c r="F23" s="171"/>
+      <c r="G23" s="171"/>
+      <c r="H23" s="171"/>
+      <c r="I23" s="171"/>
+      <c r="J23" s="171"/>
+      <c r="K23" s="171"/>
+      <c r="L23" s="171"/>
+      <c r="M23" s="171"/>
+      <c r="N23" s="171"/>
+      <c r="O23" s="171"/>
+      <c r="P23" s="171"/>
       <c r="Q23" s="16"/>
     </row>
     <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="172"/>
-      <c r="C24" s="172"/>
-      <c r="D24" s="172"/>
-      <c r="E24" s="172"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="172"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="172"/>
-      <c r="J24" s="172"/>
-      <c r="K24" s="172"/>
-      <c r="L24" s="172"/>
-      <c r="M24" s="172"/>
-      <c r="N24" s="172"/>
-      <c r="O24" s="172"/>
-      <c r="P24" s="172"/>
+      <c r="B24" s="171"/>
+      <c r="C24" s="171"/>
+      <c r="D24" s="171"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="171"/>
+      <c r="G24" s="171"/>
+      <c r="H24" s="171"/>
+      <c r="I24" s="171"/>
+      <c r="J24" s="171"/>
+      <c r="K24" s="171"/>
+      <c r="L24" s="171"/>
+      <c r="M24" s="171"/>
+      <c r="N24" s="171"/>
+      <c r="O24" s="171"/>
+      <c r="P24" s="171"/>
       <c r="Q24" s="16"/>
     </row>
     <row r="25" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="172"/>
-      <c r="F25" s="172"/>
-      <c r="G25" s="172"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="172"/>
-      <c r="J25" s="172"/>
-      <c r="K25" s="172"/>
-      <c r="L25" s="172"/>
-      <c r="M25" s="172"/>
-      <c r="N25" s="172"/>
-      <c r="O25" s="172"/>
-      <c r="P25" s="172"/>
+      <c r="B25" s="171"/>
+      <c r="C25" s="171"/>
+      <c r="D25" s="171"/>
+      <c r="E25" s="171"/>
+      <c r="F25" s="171"/>
+      <c r="G25" s="171"/>
+      <c r="H25" s="171"/>
+      <c r="I25" s="171"/>
+      <c r="J25" s="171"/>
+      <c r="K25" s="171"/>
+      <c r="L25" s="171"/>
+      <c r="M25" s="171"/>
+      <c r="N25" s="171"/>
+      <c r="O25" s="171"/>
+      <c r="P25" s="171"/>
       <c r="Q25" s="16"/>
     </row>
     <row r="26" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
-      <c r="B26" s="172"/>
-      <c r="C26" s="172"/>
-      <c r="D26" s="172"/>
-      <c r="E26" s="172"/>
-      <c r="F26" s="172"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="172"/>
-      <c r="J26" s="172"/>
-      <c r="K26" s="172"/>
-      <c r="L26" s="172"/>
-      <c r="M26" s="172"/>
-      <c r="N26" s="172"/>
-      <c r="O26" s="172"/>
-      <c r="P26" s="172"/>
+      <c r="B26" s="171"/>
+      <c r="C26" s="171"/>
+      <c r="D26" s="171"/>
+      <c r="E26" s="171"/>
+      <c r="F26" s="171"/>
+      <c r="G26" s="171"/>
+      <c r="H26" s="171"/>
+      <c r="I26" s="171"/>
+      <c r="J26" s="171"/>
+      <c r="K26" s="171"/>
+      <c r="L26" s="171"/>
+      <c r="M26" s="171"/>
+      <c r="N26" s="171"/>
+      <c r="O26" s="171"/>
+      <c r="P26" s="171"/>
       <c r="Q26" s="16"/>
     </row>
     <row r="27" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
-      <c r="B27" s="172"/>
-      <c r="C27" s="172"/>
-      <c r="D27" s="172"/>
-      <c r="E27" s="172"/>
-      <c r="F27" s="172"/>
-      <c r="G27" s="172"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="172"/>
-      <c r="J27" s="172"/>
-      <c r="K27" s="172"/>
-      <c r="L27" s="172"/>
-      <c r="M27" s="172"/>
-      <c r="N27" s="172"/>
-      <c r="O27" s="172"/>
-      <c r="P27" s="172"/>
+      <c r="B27" s="171"/>
+      <c r="C27" s="171"/>
+      <c r="D27" s="171"/>
+      <c r="E27" s="171"/>
+      <c r="F27" s="171"/>
+      <c r="G27" s="171"/>
+      <c r="H27" s="171"/>
+      <c r="I27" s="171"/>
+      <c r="J27" s="171"/>
+      <c r="K27" s="171"/>
+      <c r="L27" s="171"/>
+      <c r="M27" s="171"/>
+      <c r="N27" s="171"/>
+      <c r="O27" s="171"/>
+      <c r="P27" s="171"/>
       <c r="Q27" s="16"/>
     </row>
     <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
-      <c r="B28" s="171"/>
-      <c r="C28" s="171"/>
-      <c r="D28" s="171"/>
-      <c r="E28" s="171"/>
-      <c r="F28" s="171"/>
-      <c r="G28" s="171"/>
-      <c r="H28" s="171"/>
-      <c r="I28" s="171"/>
-      <c r="J28" s="171"/>
-      <c r="K28" s="171"/>
-      <c r="L28" s="171"/>
-      <c r="M28" s="171"/>
-      <c r="N28" s="171"/>
-      <c r="O28" s="171"/>
-      <c r="P28" s="171"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="172"/>
+      <c r="E28" s="172"/>
+      <c r="F28" s="172"/>
+      <c r="G28" s="172"/>
+      <c r="H28" s="172"/>
+      <c r="I28" s="172"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="172"/>
+      <c r="L28" s="172"/>
+      <c r="M28" s="172"/>
+      <c r="N28" s="172"/>
+      <c r="O28" s="172"/>
+      <c r="P28" s="172"/>
       <c r="Q28" s="16"/>
     </row>
     <row r="29" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,386 +2587,386 @@
     </row>
     <row r="30" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
-      <c r="B30" s="105" t="s">
+      <c r="B30" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="C30" s="140"/>
+      <c r="D30" s="140"/>
       <c r="E30" s="43"/>
-      <c r="F30" s="105" t="s">
+      <c r="F30" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="106"/>
-      <c r="H30" s="107" t="s">
+      <c r="G30" s="141"/>
+      <c r="H30" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="105"/>
-      <c r="J30" s="105"/>
-      <c r="K30" s="105"/>
-      <c r="L30" s="105"/>
-      <c r="M30" s="105"/>
+      <c r="I30" s="140"/>
+      <c r="J30" s="140"/>
+      <c r="K30" s="140"/>
+      <c r="L30" s="140"/>
+      <c r="M30" s="140"/>
       <c r="N30" s="44"/>
-      <c r="O30" s="105" t="s">
+      <c r="O30" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="P30" s="105"/>
+      <c r="P30" s="140"/>
       <c r="Q30" s="45"/>
     </row>
     <row r="31" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46"/>
-      <c r="B32" s="88" t="s">
+      <c r="B32" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="88"/>
-      <c r="H32" s="88"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="M32" s="88"/>
-      <c r="N32" s="88"/>
-      <c r="O32" s="88"/>
-      <c r="P32" s="88"/>
+      <c r="C32" s="136"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="136"/>
+      <c r="G32" s="136"/>
+      <c r="H32" s="136"/>
+      <c r="I32" s="136"/>
+      <c r="J32" s="136"/>
+      <c r="K32" s="136"/>
+      <c r="L32" s="136"/>
+      <c r="M32" s="136"/>
+      <c r="N32" s="136"/>
+      <c r="O32" s="136"/>
+      <c r="P32" s="136"/>
       <c r="Q32" s="47"/>
     </row>
     <row r="33" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48"/>
-      <c r="B33" s="108" t="s">
+      <c r="B33" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="108"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="108"/>
-      <c r="F33" s="108"/>
-      <c r="G33" s="108"/>
-      <c r="H33" s="108"/>
-      <c r="I33" s="108"/>
-      <c r="J33" s="108"/>
-      <c r="K33" s="108"/>
-      <c r="L33" s="109"/>
-      <c r="M33" s="110"/>
-      <c r="N33" s="111"/>
-      <c r="O33" s="111"/>
-      <c r="P33" s="111"/>
+      <c r="C33" s="132"/>
+      <c r="D33" s="132"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="132"/>
+      <c r="G33" s="132"/>
+      <c r="H33" s="132"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="132"/>
+      <c r="K33" s="132"/>
+      <c r="L33" s="133"/>
+      <c r="M33" s="134"/>
+      <c r="N33" s="135"/>
+      <c r="O33" s="135"/>
+      <c r="P33" s="135"/>
       <c r="Q33" s="49"/>
     </row>
     <row r="34" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
-      <c r="B34" s="112" t="s">
+      <c r="B34" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="112"/>
-      <c r="H34" s="112"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="113"/>
-      <c r="M34" s="114"/>
-      <c r="N34" s="115"/>
-      <c r="O34" s="115"/>
-      <c r="P34" s="115"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="128"/>
+      <c r="K34" s="128"/>
+      <c r="L34" s="129"/>
+      <c r="M34" s="130"/>
+      <c r="N34" s="131"/>
+      <c r="O34" s="131"/>
+      <c r="P34" s="131"/>
       <c r="Q34" s="51"/>
     </row>
     <row r="35" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
-      <c r="B35" s="112" t="s">
+      <c r="B35" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="112"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="112"/>
-      <c r="H35" s="112"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="112"/>
-      <c r="K35" s="112"/>
-      <c r="L35" s="113"/>
-      <c r="M35" s="114"/>
-      <c r="N35" s="115"/>
-      <c r="O35" s="115"/>
-      <c r="P35" s="115"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="128"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="128"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="128"/>
+      <c r="L35" s="129"/>
+      <c r="M35" s="130"/>
+      <c r="N35" s="131"/>
+      <c r="O35" s="131"/>
+      <c r="P35" s="131"/>
       <c r="Q35" s="51"/>
     </row>
     <row r="36" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
-      <c r="B36" s="112" t="s">
+      <c r="B36" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="112"/>
-      <c r="H36" s="112"/>
-      <c r="I36" s="112"/>
-      <c r="J36" s="112"/>
-      <c r="K36" s="112"/>
-      <c r="L36" s="113"/>
-      <c r="M36" s="114"/>
-      <c r="N36" s="115"/>
-      <c r="O36" s="115"/>
-      <c r="P36" s="115"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="128"/>
+      <c r="G36" s="128"/>
+      <c r="H36" s="128"/>
+      <c r="I36" s="128"/>
+      <c r="J36" s="128"/>
+      <c r="K36" s="128"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="130"/>
+      <c r="N36" s="131"/>
+      <c r="O36" s="131"/>
+      <c r="P36" s="131"/>
       <c r="Q36" s="51"/>
     </row>
     <row r="37" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
-      <c r="B37" s="112" t="s">
+      <c r="B37" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="112"/>
-      <c r="D37" s="112"/>
-      <c r="E37" s="112"/>
-      <c r="F37" s="112"/>
-      <c r="G37" s="112"/>
-      <c r="H37" s="112"/>
-      <c r="I37" s="112"/>
-      <c r="J37" s="112"/>
-      <c r="K37" s="112"/>
-      <c r="L37" s="113"/>
-      <c r="M37" s="114"/>
-      <c r="N37" s="115"/>
-      <c r="O37" s="115"/>
-      <c r="P37" s="115"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="128"/>
+      <c r="E37" s="128"/>
+      <c r="F37" s="128"/>
+      <c r="G37" s="128"/>
+      <c r="H37" s="128"/>
+      <c r="I37" s="128"/>
+      <c r="J37" s="128"/>
+      <c r="K37" s="128"/>
+      <c r="L37" s="129"/>
+      <c r="M37" s="130"/>
+      <c r="N37" s="131"/>
+      <c r="O37" s="131"/>
+      <c r="P37" s="131"/>
       <c r="Q37" s="51"/>
     </row>
     <row r="38" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
-      <c r="B38" s="112" t="s">
+      <c r="B38" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="112"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="112"/>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="113"/>
-      <c r="M38" s="114"/>
-      <c r="N38" s="115"/>
-      <c r="O38" s="115"/>
-      <c r="P38" s="115"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="128"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="128"/>
+      <c r="H38" s="128"/>
+      <c r="I38" s="128"/>
+      <c r="J38" s="128"/>
+      <c r="K38" s="128"/>
+      <c r="L38" s="129"/>
+      <c r="M38" s="130"/>
+      <c r="N38" s="131"/>
+      <c r="O38" s="131"/>
+      <c r="P38" s="131"/>
       <c r="Q38" s="51"/>
     </row>
     <row r="39" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="116"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="116"/>
-      <c r="F39" s="116"/>
-      <c r="G39" s="116"/>
-      <c r="H39" s="116"/>
-      <c r="I39" s="116"/>
-      <c r="J39" s="116"/>
-      <c r="K39" s="116"/>
-      <c r="L39" s="117"/>
-      <c r="M39" s="118"/>
-      <c r="N39" s="119"/>
-      <c r="O39" s="119"/>
-      <c r="P39" s="119"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101"/>
+      <c r="H39" s="101"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="102"/>
+      <c r="M39" s="103"/>
+      <c r="N39" s="104"/>
+      <c r="O39" s="104"/>
+      <c r="P39" s="104"/>
       <c r="Q39" s="53"/>
     </row>
     <row r="40" spans="1:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:17" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="54"/>
-      <c r="B41" s="120" t="s">
+      <c r="B41" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="120"/>
-      <c r="D41" s="122" t="s">
+      <c r="C41" s="105"/>
+      <c r="D41" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="123"/>
-      <c r="F41" s="124"/>
-      <c r="G41" s="128" t="s">
+      <c r="E41" s="108"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="129"/>
-      <c r="I41" s="129"/>
-      <c r="J41" s="129"/>
-      <c r="K41" s="129"/>
-      <c r="L41" s="132" t="s">
+      <c r="H41" s="114"/>
+      <c r="I41" s="114"/>
+      <c r="J41" s="114"/>
+      <c r="K41" s="114"/>
+      <c r="L41" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="M41" s="133"/>
-      <c r="N41" s="133"/>
-      <c r="O41" s="133"/>
-      <c r="P41" s="133"/>
+      <c r="M41" s="118"/>
+      <c r="N41" s="118"/>
+      <c r="O41" s="118"/>
+      <c r="P41" s="118"/>
       <c r="Q41" s="55"/>
     </row>
     <row r="42" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
-      <c r="B42" s="121"/>
-      <c r="C42" s="121"/>
-      <c r="D42" s="125"/>
-      <c r="E42" s="126"/>
-      <c r="F42" s="127"/>
-      <c r="G42" s="130"/>
-      <c r="H42" s="131"/>
-      <c r="I42" s="131"/>
-      <c r="J42" s="131"/>
-      <c r="K42" s="131"/>
-      <c r="L42" s="134"/>
-      <c r="M42" s="135"/>
-      <c r="N42" s="135"/>
-      <c r="O42" s="135"/>
-      <c r="P42" s="135"/>
+      <c r="B42" s="106"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="110"/>
+      <c r="E42" s="111"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="115"/>
+      <c r="H42" s="116"/>
+      <c r="I42" s="116"/>
+      <c r="J42" s="116"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="119"/>
+      <c r="M42" s="120"/>
+      <c r="N42" s="120"/>
+      <c r="O42" s="120"/>
+      <c r="P42" s="120"/>
       <c r="Q42" s="57"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
-      <c r="B43" s="121"/>
-      <c r="C43" s="121"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="126"/>
-      <c r="F43" s="127"/>
-      <c r="G43" s="130"/>
-      <c r="H43" s="131"/>
-      <c r="I43" s="131"/>
-      <c r="J43" s="131"/>
-      <c r="K43" s="131"/>
-      <c r="L43" s="134"/>
-      <c r="M43" s="135"/>
-      <c r="N43" s="135"/>
-      <c r="O43" s="135"/>
-      <c r="P43" s="135"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="110"/>
+      <c r="E43" s="111"/>
+      <c r="F43" s="112"/>
+      <c r="G43" s="115"/>
+      <c r="H43" s="116"/>
+      <c r="I43" s="116"/>
+      <c r="J43" s="116"/>
+      <c r="K43" s="116"/>
+      <c r="L43" s="119"/>
+      <c r="M43" s="120"/>
+      <c r="N43" s="120"/>
+      <c r="O43" s="120"/>
+      <c r="P43" s="120"/>
       <c r="Q43" s="57"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="56"/>
-      <c r="B44" s="121"/>
-      <c r="C44" s="121"/>
-      <c r="D44" s="136"/>
-      <c r="E44" s="137"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="139"/>
-      <c r="H44" s="140"/>
-      <c r="I44" s="140"/>
-      <c r="J44" s="140"/>
-      <c r="K44" s="140"/>
-      <c r="L44" s="141"/>
-      <c r="M44" s="142"/>
-      <c r="N44" s="142"/>
-      <c r="O44" s="142"/>
-      <c r="P44" s="142"/>
+      <c r="B44" s="106"/>
+      <c r="C44" s="106"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="124"/>
+      <c r="H44" s="125"/>
+      <c r="I44" s="125"/>
+      <c r="J44" s="125"/>
+      <c r="K44" s="125"/>
+      <c r="L44" s="126"/>
+      <c r="M44" s="127"/>
+      <c r="N44" s="127"/>
+      <c r="O44" s="127"/>
+      <c r="P44" s="127"/>
       <c r="Q44" s="57"/>
     </row>
     <row r="45" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56"/>
-      <c r="B45" s="121"/>
-      <c r="C45" s="121"/>
-      <c r="D45" s="136"/>
-      <c r="E45" s="137"/>
-      <c r="F45" s="138"/>
-      <c r="G45" s="139"/>
-      <c r="H45" s="140"/>
-      <c r="I45" s="140"/>
-      <c r="J45" s="140"/>
-      <c r="K45" s="140"/>
-      <c r="L45" s="141"/>
-      <c r="M45" s="142"/>
-      <c r="N45" s="142"/>
-      <c r="O45" s="142"/>
-      <c r="P45" s="142"/>
+      <c r="B45" s="106"/>
+      <c r="C45" s="106"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="124"/>
+      <c r="H45" s="125"/>
+      <c r="I45" s="125"/>
+      <c r="J45" s="125"/>
+      <c r="K45" s="125"/>
+      <c r="L45" s="126"/>
+      <c r="M45" s="127"/>
+      <c r="N45" s="127"/>
+      <c r="O45" s="127"/>
+      <c r="P45" s="127"/>
       <c r="Q45" s="57"/>
     </row>
     <row r="46" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="58"/>
-      <c r="B46" s="143" t="s">
+      <c r="B46" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="143"/>
-      <c r="D46" s="144"/>
-      <c r="E46" s="145"/>
-      <c r="F46" s="146"/>
-      <c r="G46" s="147"/>
-      <c r="H46" s="148"/>
-      <c r="I46" s="148"/>
-      <c r="J46" s="148"/>
-      <c r="K46" s="148"/>
-      <c r="L46" s="149"/>
-      <c r="M46" s="150"/>
-      <c r="N46" s="150"/>
-      <c r="O46" s="150"/>
-      <c r="P46" s="150"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="91"/>
+      <c r="E46" s="92"/>
+      <c r="F46" s="93"/>
+      <c r="G46" s="94"/>
+      <c r="H46" s="95"/>
+      <c r="I46" s="95"/>
+      <c r="J46" s="95"/>
+      <c r="K46" s="95"/>
+      <c r="L46" s="96"/>
+      <c r="M46" s="97"/>
+      <c r="N46" s="97"/>
+      <c r="O46" s="97"/>
+      <c r="P46" s="97"/>
       <c r="Q46" s="59"/>
     </row>
     <row r="47" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
-      <c r="B47" s="151" t="s">
+      <c r="B47" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="151"/>
-      <c r="D47" s="152"/>
-      <c r="E47" s="153"/>
-      <c r="F47" s="154"/>
-      <c r="G47" s="155"/>
-      <c r="H47" s="156"/>
-      <c r="I47" s="156"/>
-      <c r="J47" s="156"/>
-      <c r="K47" s="156"/>
-      <c r="L47" s="157"/>
-      <c r="M47" s="158"/>
-      <c r="N47" s="158"/>
-      <c r="O47" s="158"/>
-      <c r="P47" s="158"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="83"/>
+      <c r="E47" s="84"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="98"/>
+      <c r="H47" s="87"/>
+      <c r="I47" s="87"/>
+      <c r="J47" s="87"/>
+      <c r="K47" s="87"/>
+      <c r="L47" s="99"/>
+      <c r="M47" s="100"/>
+      <c r="N47" s="100"/>
+      <c r="O47" s="100"/>
+      <c r="P47" s="100"/>
       <c r="Q47" s="62"/>
     </row>
     <row r="48" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="63"/>
-      <c r="B48" s="160" t="s">
+      <c r="B48" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="160"/>
-      <c r="D48" s="161"/>
-      <c r="E48" s="162"/>
-      <c r="F48" s="163"/>
-      <c r="G48" s="164"/>
-      <c r="H48" s="165"/>
-      <c r="I48" s="165"/>
-      <c r="J48" s="165"/>
-      <c r="K48" s="165"/>
-      <c r="L48" s="166"/>
-      <c r="M48" s="167"/>
-      <c r="N48" s="167"/>
-      <c r="O48" s="167"/>
-      <c r="P48" s="167"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="79"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="80"/>
+      <c r="M48" s="81"/>
+      <c r="N48" s="81"/>
+      <c r="O48" s="81"/>
+      <c r="P48" s="81"/>
       <c r="Q48" s="64"/>
     </row>
     <row r="49" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="61"/>
-      <c r="B49" s="151" t="s">
+      <c r="B49" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="151"/>
-      <c r="D49" s="152"/>
-      <c r="E49" s="153"/>
-      <c r="F49" s="154"/>
-      <c r="G49" s="168"/>
-      <c r="H49" s="156"/>
-      <c r="I49" s="156"/>
-      <c r="J49" s="156"/>
-      <c r="K49" s="156"/>
-      <c r="L49" s="169"/>
-      <c r="M49" s="170"/>
-      <c r="N49" s="170"/>
-      <c r="O49" s="170"/>
-      <c r="P49" s="170"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="86"/>
+      <c r="H49" s="87"/>
+      <c r="I49" s="87"/>
+      <c r="J49" s="87"/>
+      <c r="K49" s="87"/>
+      <c r="L49" s="88"/>
+      <c r="M49" s="89"/>
+      <c r="N49" s="89"/>
+      <c r="O49" s="89"/>
+      <c r="P49" s="89"/>
       <c r="Q49" s="62"/>
     </row>
     <row r="50" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2992,72 +2992,42 @@
     </row>
     <row r="51" spans="1:17" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="71"/>
-      <c r="B51" s="159" t="s">
+      <c r="B51" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="159"/>
-      <c r="D51" s="159"/>
-      <c r="E51" s="159"/>
-      <c r="F51" s="159"/>
-      <c r="G51" s="159"/>
-      <c r="H51" s="159"/>
-      <c r="I51" s="159"/>
-      <c r="J51" s="159"/>
-      <c r="K51" s="159"/>
-      <c r="L51" s="159"/>
-      <c r="M51" s="159"/>
-      <c r="N51" s="159"/>
-      <c r="O51" s="159"/>
-      <c r="P51" s="159"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="73"/>
+      <c r="F51" s="73"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="73"/>
+      <c r="I51" s="73"/>
+      <c r="J51" s="73"/>
+      <c r="K51" s="73"/>
+      <c r="L51" s="73"/>
+      <c r="M51" s="73"/>
+      <c r="N51" s="73"/>
+      <c r="O51" s="73"/>
+      <c r="P51" s="73"/>
       <c r="Q51" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="B51:P51"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="L48:P48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="G49:K49"/>
-    <mergeCell ref="L49:P49"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="L46:P46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="L47:P47"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D41:F43"/>
-    <mergeCell ref="G41:K43"/>
-    <mergeCell ref="L41:P43"/>
-    <mergeCell ref="D44:F45"/>
-    <mergeCell ref="G44:K45"/>
-    <mergeCell ref="L44:P45"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="M37:P37"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="B32:P32"/>
-    <mergeCell ref="A22:Q22"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="B23:P28"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="D1:Q1"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D3:Q3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="P11:Q11"/>
     <mergeCell ref="B21:P21"/>
     <mergeCell ref="B12:P13"/>
     <mergeCell ref="B14:P14"/>
@@ -3070,21 +3040,51 @@
     <mergeCell ref="L17:P17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="L18:P18"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="D1:Q1"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D3:Q3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="A22:Q22"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="B23:P28"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="D41:F43"/>
+    <mergeCell ref="G41:K43"/>
+    <mergeCell ref="L41:P43"/>
+    <mergeCell ref="D44:F45"/>
+    <mergeCell ref="G44:K45"/>
+    <mergeCell ref="L44:P45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="L46:P46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="L47:P47"/>
+    <mergeCell ref="B51:P51"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="G48:K48"/>
+    <mergeCell ref="L48:P48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="G49:K49"/>
+    <mergeCell ref="L49:P49"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
@@ -3096,12 +3096,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D262036FF67A5D43BF6E290DEB360352" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c503d2a7b448377a6cc9e75158e3af5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e744003-367c-4be8-bc40-2385cb622540" xmlns:ns3="0930cf9b-719b-4120-8db4-f84070340397" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9cea96fa3cc1abdf61d90e2bf9fac8d2" ns2:_="" ns3:_="">
     <xsd:import namespace="4e744003-367c-4be8-bc40-2385cb622540"/>
@@ -3318,6 +3312,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3328,23 +3328,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3DC5811-E2D9-4774-B143-A47CE40C3F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3363,6 +3346,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
w1 w2 fecm bug fixes
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>PERFORMANCE-BASED CONTRACT FOR THE LONG-TERM MANAGEMENT AND MAINTENANCE OF STATE ROADS [JALANRAYA NEGERI (JRN)] IN SARAWAK - PACKAGE 4  (MIRI DIVISION)</t>
   </si>
@@ -134,54 +134,6 @@
   </si>
   <si>
     <t>General and Preliminaries</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Consultancy Fees </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+ Government Tax @       % (If any)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Survey Works </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+ Government Tax @        % (If any)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Site Investigation </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+ Government Tax @         % (If any)</t>
-    </r>
-  </si>
-  <si>
-    <t>Any other cost:</t>
   </si>
   <si>
     <t>Estimated Total Cost</t>
@@ -255,33 +207,25 @@
     <t>Date:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Name for this Instructed Work Proposal: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(to be given by S.O. / S.O.'s Rep.)</t>
-    </r>
-  </si>
-  <si>
     <t>PROPOSED REHABILATION FOR SLOPE AT CH28+970, Q3178 JALAN MIRI MARUDI</t>
   </si>
   <si>
     <t xml:space="preserve">CONTRACT NO: </t>
+  </si>
+  <si>
+    <t>Consultancy Fees + Government Tax</t>
+  </si>
+  <si>
+    <t>Name for this Instructed Work Proposal:</t>
+  </si>
+  <si>
+    <t>% (if any)</t>
+  </si>
+  <si>
+    <t>Survey Works  +  Government Tax</t>
+  </si>
+  <si>
+    <t>Site Investigation +  Government Tax</t>
   </si>
 </sst>
 </file>
@@ -293,7 +237,7 @@
     <numFmt numFmtId="165" formatCode="_-&quot;RM&quot;* #,##0.00_-;\-&quot;RM&quot;* #,##0.00_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="#,###.00"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,14 +398,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -925,7 +861,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1082,17 +1018,12 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1144,6 +1075,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1258,18 +1192,18 @@
     <xf numFmtId="166" fontId="21" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1282,6 +1216,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1303,6 +1240,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1386,12 +1329,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1986,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,64 +1943,64 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="163" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="164"/>
+      <c r="D1" s="166" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="167"/>
     </row>
     <row r="2" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="165" t="s">
+      <c r="D2" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
-      <c r="Q2" s="167"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="170"/>
     </row>
     <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="168" t="s">
+      <c r="D3" s="171" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
-      <c r="J3" s="168"/>
-      <c r="K3" s="168"/>
-      <c r="L3" s="168"/>
-      <c r="M3" s="168"/>
-      <c r="N3" s="168"/>
-      <c r="O3" s="168"/>
-      <c r="P3" s="168"/>
-      <c r="Q3" s="169"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171"/>
+      <c r="N3" s="171"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="172"/>
     </row>
     <row r="4" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -2105,16 +2042,16 @@
     </row>
     <row r="6" spans="1:18" ht="2.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="170"/>
-      <c r="C6" s="170"/>
+      <c r="B6" s="173"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="170"/>
-      <c r="K6" s="170"/>
+      <c r="J6" s="173"/>
+      <c r="K6" s="173"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -2124,25 +2061,25 @@
     </row>
     <row r="7" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="157"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="156" t="s">
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="160"/>
+      <c r="F7" s="160"/>
+      <c r="G7" s="160"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="156"/>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="158"/>
-      <c r="O7" s="158"/>
-      <c r="P7" s="158"/>
+      <c r="K7" s="159"/>
+      <c r="L7" s="161"/>
+      <c r="M7" s="161"/>
+      <c r="N7" s="161"/>
+      <c r="O7" s="161"/>
+      <c r="P7" s="161"/>
       <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.3">
@@ -2166,25 +2103,25 @@
     </row>
     <row r="9" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
-      <c r="B9" s="156" t="s">
+      <c r="B9" s="159" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="156" t="s">
+      <c r="C9" s="159"/>
+      <c r="D9" s="159"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="160"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="156"/>
-      <c r="L9" s="158"/>
-      <c r="M9" s="158"/>
-      <c r="N9" s="158"/>
-      <c r="O9" s="158"/>
-      <c r="P9" s="158"/>
+      <c r="K9" s="159"/>
+      <c r="L9" s="161"/>
+      <c r="M9" s="161"/>
+      <c r="N9" s="161"/>
+      <c r="O9" s="161"/>
+      <c r="P9" s="161"/>
       <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="1:18" ht="1.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2218,70 +2155,70 @@
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="159"/>
-      <c r="M11" s="159"/>
+      <c r="L11" s="162"/>
+      <c r="M11" s="162"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="160"/>
-      <c r="Q11" s="161"/>
+      <c r="P11" s="163"/>
+      <c r="Q11" s="164"/>
     </row>
     <row r="12" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="143"/>
-      <c r="D12" s="143"/>
-      <c r="E12" s="143"/>
-      <c r="F12" s="143"/>
-      <c r="G12" s="143"/>
-      <c r="H12" s="143"/>
-      <c r="I12" s="143"/>
-      <c r="J12" s="143"/>
-      <c r="K12" s="143"/>
-      <c r="L12" s="143"/>
-      <c r="M12" s="143"/>
-      <c r="N12" s="143"/>
-      <c r="O12" s="143"/>
-      <c r="P12" s="143"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="146"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="146"/>
+      <c r="M12" s="146"/>
+      <c r="N12" s="146"/>
+      <c r="O12" s="146"/>
+      <c r="P12" s="146"/>
       <c r="Q12" s="23"/>
     </row>
     <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="144"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="144"/>
-      <c r="E13" s="144"/>
-      <c r="F13" s="144"/>
-      <c r="G13" s="144"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="144"/>
-      <c r="J13" s="144"/>
-      <c r="K13" s="144"/>
-      <c r="L13" s="144"/>
-      <c r="M13" s="144"/>
-      <c r="N13" s="144"/>
-      <c r="O13" s="144"/>
-      <c r="P13" s="144"/>
+      <c r="B13" s="147"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="147"/>
+      <c r="K13" s="147"/>
+      <c r="L13" s="147"/>
+      <c r="M13" s="147"/>
+      <c r="N13" s="147"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="147"/>
       <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:18" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="145"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="145"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="145"/>
-      <c r="G14" s="145"/>
-      <c r="H14" s="145"/>
-      <c r="I14" s="145"/>
-      <c r="J14" s="145"/>
-      <c r="K14" s="145"/>
-      <c r="L14" s="145"/>
-      <c r="M14" s="145"/>
-      <c r="N14" s="145"/>
-      <c r="O14" s="145"/>
-      <c r="P14" s="145"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="148"/>
+      <c r="D14" s="148"/>
+      <c r="E14" s="148"/>
+      <c r="F14" s="148"/>
+      <c r="G14" s="148"/>
+      <c r="H14" s="148"/>
+      <c r="I14" s="148"/>
+      <c r="J14" s="148"/>
+      <c r="K14" s="148"/>
+      <c r="L14" s="148"/>
+      <c r="M14" s="148"/>
+      <c r="N14" s="148"/>
+      <c r="O14" s="148"/>
+      <c r="P14" s="148"/>
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2308,67 +2245,67 @@
     </row>
     <row r="16" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="146"/>
-      <c r="D16" s="147"/>
-      <c r="E16" s="147"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="147"/>
-      <c r="H16" s="146" t="s">
+      <c r="C16" s="149"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="150"/>
+      <c r="F16" s="150"/>
+      <c r="G16" s="150"/>
+      <c r="H16" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="146"/>
-      <c r="J16" s="146"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="148"/>
-      <c r="M16" s="148"/>
-      <c r="N16" s="148"/>
-      <c r="O16" s="148"/>
-      <c r="P16" s="148"/>
+      <c r="I16" s="149"/>
+      <c r="J16" s="149"/>
+      <c r="K16" s="149"/>
+      <c r="L16" s="151"/>
+      <c r="M16" s="151"/>
+      <c r="N16" s="151"/>
+      <c r="O16" s="151"/>
+      <c r="P16" s="151"/>
       <c r="Q16" s="30"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="149" t="s">
+      <c r="B17" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="149"/>
-      <c r="D17" s="150"/>
-      <c r="E17" s="150"/>
-      <c r="F17" s="150"/>
-      <c r="G17" s="150"/>
-      <c r="H17" s="150"/>
-      <c r="I17" s="150"/>
-      <c r="J17" s="150"/>
-      <c r="K17" s="150"/>
-      <c r="L17" s="152" t="s">
+      <c r="C17" s="152"/>
+      <c r="D17" s="153"/>
+      <c r="E17" s="153"/>
+      <c r="F17" s="153"/>
+      <c r="G17" s="153"/>
+      <c r="H17" s="153"/>
+      <c r="I17" s="153"/>
+      <c r="J17" s="153"/>
+      <c r="K17" s="153"/>
+      <c r="L17" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="153"/>
-      <c r="N17" s="153"/>
-      <c r="O17" s="153"/>
-      <c r="P17" s="153"/>
+      <c r="M17" s="156"/>
+      <c r="N17" s="156"/>
+      <c r="O17" s="156"/>
+      <c r="P17" s="156"/>
       <c r="Q17" s="32"/>
     </row>
     <row r="18" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="149"/>
-      <c r="C18" s="149"/>
-      <c r="D18" s="151"/>
-      <c r="E18" s="151"/>
-      <c r="F18" s="151"/>
-      <c r="G18" s="151"/>
-      <c r="H18" s="151"/>
-      <c r="I18" s="151"/>
-      <c r="J18" s="151"/>
-      <c r="K18" s="151"/>
-      <c r="L18" s="154"/>
-      <c r="M18" s="155"/>
-      <c r="N18" s="155"/>
-      <c r="O18" s="155"/>
-      <c r="P18" s="155"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="152"/>
+      <c r="D18" s="154"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="154"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
+      <c r="K18" s="154"/>
+      <c r="L18" s="157"/>
+      <c r="M18" s="158"/>
+      <c r="N18" s="158"/>
+      <c r="O18" s="158"/>
+      <c r="P18" s="158"/>
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:18" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2411,159 +2348,159 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="136"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="136"/>
-      <c r="H21" s="136"/>
-      <c r="I21" s="136"/>
-      <c r="J21" s="136"/>
-      <c r="K21" s="136"/>
-      <c r="L21" s="136"/>
-      <c r="M21" s="136"/>
-      <c r="N21" s="136"/>
-      <c r="O21" s="136"/>
-      <c r="P21" s="136"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="137"/>
+      <c r="H21" s="137"/>
+      <c r="I21" s="137"/>
+      <c r="J21" s="137"/>
+      <c r="K21" s="137"/>
+      <c r="L21" s="137"/>
+      <c r="M21" s="137"/>
+      <c r="N21" s="137"/>
+      <c r="O21" s="137"/>
+      <c r="P21" s="137"/>
       <c r="Q21" s="27"/>
       <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="137" t="s">
+      <c r="A22" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="138"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="138"/>
-      <c r="I22" s="138"/>
-      <c r="J22" s="138"/>
-      <c r="K22" s="138"/>
-      <c r="L22" s="138"/>
-      <c r="M22" s="138"/>
-      <c r="N22" s="138"/>
-      <c r="O22" s="138"/>
-      <c r="P22" s="138"/>
-      <c r="Q22" s="139"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="139"/>
+      <c r="J22" s="139"/>
+      <c r="K22" s="139"/>
+      <c r="L22" s="139"/>
+      <c r="M22" s="139"/>
+      <c r="N22" s="139"/>
+      <c r="O22" s="139"/>
+      <c r="P22" s="139"/>
+      <c r="Q22" s="140"/>
     </row>
     <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
-      <c r="B23" s="171"/>
-      <c r="C23" s="171"/>
-      <c r="D23" s="171"/>
-      <c r="E23" s="171"/>
-      <c r="F23" s="171"/>
-      <c r="G23" s="171"/>
-      <c r="H23" s="171"/>
-      <c r="I23" s="171"/>
-      <c r="J23" s="171"/>
-      <c r="K23" s="171"/>
-      <c r="L23" s="171"/>
-      <c r="M23" s="171"/>
-      <c r="N23" s="171"/>
-      <c r="O23" s="171"/>
-      <c r="P23" s="171"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="144"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="144"/>
+      <c r="J23" s="144"/>
+      <c r="K23" s="144"/>
+      <c r="L23" s="144"/>
+      <c r="M23" s="144"/>
+      <c r="N23" s="144"/>
+      <c r="O23" s="144"/>
+      <c r="P23" s="144"/>
       <c r="Q23" s="16"/>
     </row>
     <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="171"/>
-      <c r="C24" s="171"/>
-      <c r="D24" s="171"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="171"/>
-      <c r="G24" s="171"/>
-      <c r="H24" s="171"/>
-      <c r="I24" s="171"/>
-      <c r="J24" s="171"/>
-      <c r="K24" s="171"/>
-      <c r="L24" s="171"/>
-      <c r="M24" s="171"/>
-      <c r="N24" s="171"/>
-      <c r="O24" s="171"/>
-      <c r="P24" s="171"/>
+      <c r="B24" s="144"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
+      <c r="J24" s="144"/>
+      <c r="K24" s="144"/>
+      <c r="L24" s="144"/>
+      <c r="M24" s="144"/>
+      <c r="N24" s="144"/>
+      <c r="O24" s="144"/>
+      <c r="P24" s="144"/>
       <c r="Q24" s="16"/>
     </row>
     <row r="25" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
-      <c r="B25" s="171"/>
-      <c r="C25" s="171"/>
-      <c r="D25" s="171"/>
-      <c r="E25" s="171"/>
-      <c r="F25" s="171"/>
-      <c r="G25" s="171"/>
-      <c r="H25" s="171"/>
-      <c r="I25" s="171"/>
-      <c r="J25" s="171"/>
-      <c r="K25" s="171"/>
-      <c r="L25" s="171"/>
-      <c r="M25" s="171"/>
-      <c r="N25" s="171"/>
-      <c r="O25" s="171"/>
-      <c r="P25" s="171"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="144"/>
+      <c r="G25" s="144"/>
+      <c r="H25" s="144"/>
+      <c r="I25" s="144"/>
+      <c r="J25" s="144"/>
+      <c r="K25" s="144"/>
+      <c r="L25" s="144"/>
+      <c r="M25" s="144"/>
+      <c r="N25" s="144"/>
+      <c r="O25" s="144"/>
+      <c r="P25" s="144"/>
       <c r="Q25" s="16"/>
     </row>
     <row r="26" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
-      <c r="B26" s="171"/>
-      <c r="C26" s="171"/>
-      <c r="D26" s="171"/>
-      <c r="E26" s="171"/>
-      <c r="F26" s="171"/>
-      <c r="G26" s="171"/>
-      <c r="H26" s="171"/>
-      <c r="I26" s="171"/>
-      <c r="J26" s="171"/>
-      <c r="K26" s="171"/>
-      <c r="L26" s="171"/>
-      <c r="M26" s="171"/>
-      <c r="N26" s="171"/>
-      <c r="O26" s="171"/>
-      <c r="P26" s="171"/>
+      <c r="B26" s="144"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="144"/>
+      <c r="K26" s="144"/>
+      <c r="L26" s="144"/>
+      <c r="M26" s="144"/>
+      <c r="N26" s="144"/>
+      <c r="O26" s="144"/>
+      <c r="P26" s="144"/>
       <c r="Q26" s="16"/>
     </row>
     <row r="27" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
-      <c r="B27" s="171"/>
-      <c r="C27" s="171"/>
-      <c r="D27" s="171"/>
-      <c r="E27" s="171"/>
-      <c r="F27" s="171"/>
-      <c r="G27" s="171"/>
-      <c r="H27" s="171"/>
-      <c r="I27" s="171"/>
-      <c r="J27" s="171"/>
-      <c r="K27" s="171"/>
-      <c r="L27" s="171"/>
-      <c r="M27" s="171"/>
-      <c r="N27" s="171"/>
-      <c r="O27" s="171"/>
-      <c r="P27" s="171"/>
+      <c r="B27" s="144"/>
+      <c r="C27" s="144"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="144"/>
+      <c r="F27" s="144"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="144"/>
+      <c r="I27" s="144"/>
+      <c r="J27" s="144"/>
+      <c r="K27" s="144"/>
+      <c r="L27" s="144"/>
+      <c r="M27" s="144"/>
+      <c r="N27" s="144"/>
+      <c r="O27" s="144"/>
+      <c r="P27" s="144"/>
       <c r="Q27" s="16"/>
     </row>
     <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="172"/>
-      <c r="D28" s="172"/>
-      <c r="E28" s="172"/>
-      <c r="F28" s="172"/>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="172"/>
-      <c r="J28" s="172"/>
-      <c r="K28" s="172"/>
-      <c r="L28" s="172"/>
-      <c r="M28" s="172"/>
-      <c r="N28" s="172"/>
-      <c r="O28" s="172"/>
-      <c r="P28" s="172"/>
+      <c r="B28" s="145"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
+      <c r="K28" s="145"/>
+      <c r="L28" s="145"/>
+      <c r="M28" s="145"/>
+      <c r="N28" s="145"/>
+      <c r="O28" s="145"/>
+      <c r="P28" s="145"/>
       <c r="Q28" s="16"/>
     </row>
     <row r="29" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,51 +2524,51 @@
     </row>
     <row r="30" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
-      <c r="B30" s="140" t="s">
+      <c r="B30" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="140"/>
-      <c r="D30" s="140"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="141"/>
       <c r="E30" s="43"/>
-      <c r="F30" s="140" t="s">
+      <c r="F30" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="141"/>
-      <c r="H30" s="142" t="s">
+      <c r="G30" s="142"/>
+      <c r="H30" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="140"/>
-      <c r="J30" s="140"/>
-      <c r="K30" s="140"/>
-      <c r="L30" s="140"/>
-      <c r="M30" s="140"/>
+      <c r="I30" s="141"/>
+      <c r="J30" s="141"/>
+      <c r="K30" s="141"/>
+      <c r="L30" s="141"/>
+      <c r="M30" s="141"/>
       <c r="N30" s="44"/>
-      <c r="O30" s="140" t="s">
+      <c r="O30" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="P30" s="140"/>
+      <c r="P30" s="141"/>
       <c r="Q30" s="45"/>
     </row>
     <row r="31" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46"/>
-      <c r="B32" s="136" t="s">
+      <c r="B32" s="137" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="136"/>
-      <c r="D32" s="136"/>
-      <c r="E32" s="136"/>
-      <c r="F32" s="136"/>
-      <c r="G32" s="136"/>
-      <c r="H32" s="136"/>
-      <c r="I32" s="136"/>
-      <c r="J32" s="136"/>
-      <c r="K32" s="136"/>
-      <c r="L32" s="136"/>
-      <c r="M32" s="136"/>
-      <c r="N32" s="136"/>
-      <c r="O32" s="136"/>
-      <c r="P32" s="136"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="137"/>
+      <c r="E32" s="137"/>
+      <c r="F32" s="137"/>
+      <c r="G32" s="137"/>
+      <c r="H32" s="137"/>
+      <c r="I32" s="137"/>
+      <c r="J32" s="137"/>
+      <c r="K32" s="137"/>
+      <c r="L32" s="137"/>
+      <c r="M32" s="137"/>
+      <c r="N32" s="137"/>
+      <c r="O32" s="137"/>
+      <c r="P32" s="137"/>
       <c r="Q32" s="47"/>
     </row>
     <row r="33" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2657,113 +2594,117 @@
     </row>
     <row r="34" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
-      <c r="B34" s="128" t="s">
+      <c r="B34" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="128"/>
-      <c r="D34" s="128"/>
-      <c r="E34" s="128"/>
-      <c r="F34" s="128"/>
-      <c r="G34" s="128"/>
-      <c r="H34" s="128"/>
-      <c r="I34" s="128"/>
-      <c r="J34" s="128"/>
-      <c r="K34" s="128"/>
-      <c r="L34" s="129"/>
-      <c r="M34" s="130"/>
-      <c r="N34" s="131"/>
-      <c r="O34" s="131"/>
-      <c r="P34" s="131"/>
+      <c r="C34" s="130"/>
+      <c r="D34" s="130"/>
+      <c r="E34" s="130"/>
+      <c r="F34" s="130"/>
+      <c r="G34" s="130"/>
+      <c r="H34" s="130"/>
+      <c r="I34" s="130"/>
+      <c r="J34" s="130"/>
+      <c r="K34" s="130"/>
+      <c r="L34" s="131"/>
+      <c r="M34" s="128"/>
+      <c r="N34" s="129"/>
+      <c r="O34" s="129"/>
+      <c r="P34" s="129"/>
       <c r="Q34" s="51"/>
     </row>
     <row r="35" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
-      <c r="B35" s="128" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="128"/>
-      <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="128"/>
-      <c r="G35" s="128"/>
-      <c r="H35" s="128"/>
-      <c r="I35" s="128"/>
-      <c r="J35" s="128"/>
-      <c r="K35" s="128"/>
-      <c r="L35" s="129"/>
-      <c r="M35" s="130"/>
-      <c r="N35" s="131"/>
-      <c r="O35" s="131"/>
-      <c r="P35" s="131"/>
+      <c r="B35" s="136" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="136"/>
+      <c r="D35" s="136"/>
+      <c r="E35" s="136"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="130" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="130"/>
+      <c r="I35" s="130"/>
+      <c r="J35" s="130"/>
+      <c r="K35" s="130"/>
+      <c r="L35" s="131"/>
+      <c r="M35" s="128"/>
+      <c r="N35" s="129"/>
+      <c r="O35" s="129"/>
+      <c r="P35" s="129"/>
       <c r="Q35" s="51"/>
     </row>
     <row r="36" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
-      <c r="B36" s="128" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="128"/>
-      <c r="D36" s="128"/>
-      <c r="E36" s="128"/>
-      <c r="F36" s="128"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="128"/>
-      <c r="I36" s="128"/>
-      <c r="J36" s="128"/>
-      <c r="K36" s="128"/>
-      <c r="L36" s="129"/>
-      <c r="M36" s="130"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="131"/>
-      <c r="P36" s="131"/>
+      <c r="B36" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="130"/>
+      <c r="D36" s="130"/>
+      <c r="E36" s="130"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="130" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="130"/>
+      <c r="I36" s="130"/>
+      <c r="J36" s="130"/>
+      <c r="K36" s="130"/>
+      <c r="L36" s="131"/>
+      <c r="M36" s="128"/>
+      <c r="N36" s="129"/>
+      <c r="O36" s="129"/>
+      <c r="P36" s="129"/>
       <c r="Q36" s="51"/>
     </row>
     <row r="37" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
-      <c r="B37" s="128" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="128"/>
-      <c r="D37" s="128"/>
-      <c r="E37" s="128"/>
-      <c r="F37" s="128"/>
-      <c r="G37" s="128"/>
-      <c r="H37" s="128"/>
-      <c r="I37" s="128"/>
-      <c r="J37" s="128"/>
-      <c r="K37" s="128"/>
-      <c r="L37" s="129"/>
-      <c r="M37" s="130"/>
-      <c r="N37" s="131"/>
-      <c r="O37" s="131"/>
-      <c r="P37" s="131"/>
+      <c r="B37" s="130" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="130"/>
+      <c r="D37" s="130"/>
+      <c r="E37" s="130"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="130" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="130"/>
+      <c r="I37" s="130"/>
+      <c r="J37" s="130"/>
+      <c r="K37" s="130"/>
+      <c r="L37" s="131"/>
+      <c r="M37" s="128"/>
+      <c r="N37" s="129"/>
+      <c r="O37" s="129"/>
+      <c r="P37" s="129"/>
       <c r="Q37" s="51"/>
     </row>
     <row r="38" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
-      <c r="B38" s="128" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="128"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="128"/>
-      <c r="F38" s="128"/>
-      <c r="G38" s="128"/>
-      <c r="H38" s="128"/>
-      <c r="I38" s="128"/>
-      <c r="J38" s="128"/>
-      <c r="K38" s="128"/>
-      <c r="L38" s="129"/>
-      <c r="M38" s="130"/>
-      <c r="N38" s="131"/>
-      <c r="O38" s="131"/>
-      <c r="P38" s="131"/>
+      <c r="B38" s="130"/>
+      <c r="C38" s="130"/>
+      <c r="D38" s="130"/>
+      <c r="E38" s="130"/>
+      <c r="F38" s="130"/>
+      <c r="G38" s="130"/>
+      <c r="H38" s="130"/>
+      <c r="I38" s="130"/>
+      <c r="J38" s="130"/>
+      <c r="K38" s="130"/>
+      <c r="L38" s="131"/>
+      <c r="M38" s="128"/>
+      <c r="N38" s="129"/>
+      <c r="O38" s="129"/>
+      <c r="P38" s="129"/>
       <c r="Q38" s="51"/>
     </row>
     <row r="39" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
       <c r="B39" s="101" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C39" s="101"/>
       <c r="D39" s="101"/>
@@ -2785,23 +2726,23 @@
     <row r="41" spans="1:17" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="54"/>
       <c r="B41" s="105" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C41" s="105"/>
       <c r="D41" s="107" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E41" s="108"/>
       <c r="F41" s="109"/>
       <c r="G41" s="113" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H41" s="114"/>
       <c r="I41" s="114"/>
       <c r="J41" s="114"/>
       <c r="K41" s="114"/>
       <c r="L41" s="117" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M41" s="118"/>
       <c r="N41" s="118"/>
@@ -2888,7 +2829,7 @@
     <row r="46" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="58"/>
       <c r="B46" s="90" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C46" s="90"/>
       <c r="D46" s="91"/>
@@ -2908,18 +2849,18 @@
     </row>
     <row r="47" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
-      <c r="B47" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="82"/>
-      <c r="D47" s="83"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="85"/>
+      <c r="B47" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="81"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="84"/>
       <c r="G47" s="98"/>
-      <c r="H47" s="87"/>
-      <c r="I47" s="87"/>
-      <c r="J47" s="87"/>
-      <c r="K47" s="87"/>
+      <c r="H47" s="86"/>
+      <c r="I47" s="86"/>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86"/>
       <c r="L47" s="99"/>
       <c r="M47" s="100"/>
       <c r="N47" s="100"/>
@@ -2929,90 +2870,90 @@
     </row>
     <row r="48" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="63"/>
-      <c r="B48" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="74"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="80"/>
-      <c r="M48" s="81"/>
-      <c r="N48" s="81"/>
-      <c r="O48" s="81"/>
-      <c r="P48" s="81"/>
+      <c r="B48" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="73"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="75"/>
+      <c r="F48" s="76"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="78"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="80"/>
+      <c r="N48" s="80"/>
+      <c r="O48" s="80"/>
+      <c r="P48" s="80"/>
       <c r="Q48" s="64"/>
     </row>
     <row r="49" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="61"/>
-      <c r="B49" s="82" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="82"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="84"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="86"/>
-      <c r="H49" s="87"/>
-      <c r="I49" s="87"/>
-      <c r="J49" s="87"/>
-      <c r="K49" s="87"/>
-      <c r="L49" s="88"/>
-      <c r="M49" s="89"/>
-      <c r="N49" s="89"/>
-      <c r="O49" s="89"/>
-      <c r="P49" s="89"/>
+      <c r="B49" s="81" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="81"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="85"/>
+      <c r="H49" s="86"/>
+      <c r="I49" s="86"/>
+      <c r="J49" s="86"/>
+      <c r="K49" s="86"/>
+      <c r="L49" s="87"/>
+      <c r="M49" s="88"/>
+      <c r="N49" s="88"/>
+      <c r="O49" s="88"/>
+      <c r="P49" s="88"/>
       <c r="Q49" s="62"/>
     </row>
     <row r="50" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="65"/>
-      <c r="B50" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="68"/>
-      <c r="J50" s="68"/>
-      <c r="K50" s="68"/>
-      <c r="L50" s="69"/>
-      <c r="M50" s="69"/>
-      <c r="N50" s="69"/>
-      <c r="O50" s="69"/>
-      <c r="P50" s="69"/>
-      <c r="Q50" s="70"/>
+      <c r="B50" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="89"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="67"/>
+      <c r="N50" s="67"/>
+      <c r="O50" s="67"/>
+      <c r="P50" s="67"/>
+      <c r="Q50" s="68"/>
     </row>
     <row r="51" spans="1:17" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="71"/>
-      <c r="B51" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="73"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="73"/>
-      <c r="I51" s="73"/>
-      <c r="J51" s="73"/>
-      <c r="K51" s="73"/>
-      <c r="L51" s="73"/>
-      <c r="M51" s="73"/>
-      <c r="N51" s="73"/>
-      <c r="O51" s="73"/>
-      <c r="P51" s="73"/>
-      <c r="Q51" s="72"/>
+      <c r="A51" s="69"/>
+      <c r="B51" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="72"/>
+      <c r="G51" s="72"/>
+      <c r="H51" s="72"/>
+      <c r="I51" s="72"/>
+      <c r="J51" s="72"/>
+      <c r="K51" s="72"/>
+      <c r="L51" s="72"/>
+      <c r="M51" s="72"/>
+      <c r="N51" s="72"/>
+      <c r="O51" s="72"/>
+      <c r="P51" s="72"/>
+      <c r="Q51" s="70"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="76">
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="J7:K7"/>
@@ -3051,14 +2992,17 @@
     <mergeCell ref="M33:P33"/>
     <mergeCell ref="B34:L34"/>
     <mergeCell ref="M34:P34"/>
-    <mergeCell ref="B35:L35"/>
     <mergeCell ref="M35:P35"/>
-    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="G35:L35"/>
     <mergeCell ref="M36:P36"/>
-    <mergeCell ref="B37:L37"/>
     <mergeCell ref="M37:P37"/>
     <mergeCell ref="B38:L38"/>
     <mergeCell ref="M38:P38"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="G36:L36"/>
+    <mergeCell ref="G37:L37"/>
     <mergeCell ref="B39:L39"/>
     <mergeCell ref="M39:P39"/>
     <mergeCell ref="B41:C45"/>
@@ -3085,6 +3029,7 @@
     <mergeCell ref="D49:F49"/>
     <mergeCell ref="G49:K49"/>
     <mergeCell ref="L49:P49"/>
+    <mergeCell ref="B50:F50"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
@@ -3096,6 +3041,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D262036FF67A5D43BF6E290DEB360352" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c503d2a7b448377a6cc9e75158e3af5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e744003-367c-4be8-bc40-2385cb622540" xmlns:ns3="0930cf9b-719b-4120-8db4-f84070340397" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9cea96fa3cc1abdf61d90e2bf9fac8d2" ns2:_="" ns3:_="">
     <xsd:import namespace="4e744003-367c-4be8-bc40-2385cb622540"/>
@@ -3312,22 +3272,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3DC5811-E2D9-4774-B143-A47CE40C3F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3344,29 +3314,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
demo changes and jira fixes
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW1.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>PERFORMANCE-BASED CONTRACT FOR THE LONG-TERM MANAGEMENT AND MAINTENANCE OF STATE ROADS [JALANRAYA NEGERI (JRN)] IN SARAWAK - PACKAGE 4  (MIRI DIVISION)</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Date:</t>
-  </si>
-  <si>
-    <t>PROPOSED REHABILATION FOR SLOPE AT CH28+970, Q3178 JALAN MIRI MARUDI</t>
   </si>
   <si>
     <t xml:space="preserve">CONTRACT NO: </t>
@@ -1024,6 +1021,273 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1051,24 +1315,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1077,258 +1326,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1369,7 +1366,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FA6B1FE-CE21-4599-9673-10530AEDAF91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7FA6B1FE-CE21-4599-9673-10530AEDAF91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1419,7 +1416,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{111F2E8A-CA78-40A1-B599-4BB69C13CA1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{111F2E8A-CA78-40A1-B599-4BB69C13CA1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1498,7 +1495,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42CB9192-A308-4EC5-89B8-8FC3409B7B5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{42CB9192-A308-4EC5-89B8-8FC3409B7B5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1924,7 +1921,7 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:E36"/>
+      <selection activeCell="B51" sqref="B51:P51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,64 +1940,64 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="166" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="167"/>
+      <c r="D1" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="77"/>
     </row>
     <row r="2" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="169"/>
-      <c r="L2" s="169"/>
-      <c r="M2" s="169"/>
-      <c r="N2" s="169"/>
-      <c r="O2" s="169"/>
-      <c r="P2" s="169"/>
-      <c r="Q2" s="170"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="80"/>
     </row>
     <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="171" t="s">
+      <c r="D3" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
-      <c r="I3" s="171"/>
-      <c r="J3" s="171"/>
-      <c r="K3" s="171"/>
-      <c r="L3" s="171"/>
-      <c r="M3" s="171"/>
-      <c r="N3" s="171"/>
-      <c r="O3" s="171"/>
-      <c r="P3" s="171"/>
-      <c r="Q3" s="172"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="82"/>
     </row>
     <row r="4" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -2042,16 +2039,16 @@
     </row>
     <row r="6" spans="1:18" ht="2.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="173"/>
-      <c r="C6" s="173"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="173"/>
-      <c r="K6" s="173"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -2061,25 +2058,25 @@
     </row>
     <row r="7" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="160"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="159" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="159"/>
-      <c r="L7" s="161"/>
-      <c r="M7" s="161"/>
-      <c r="N7" s="161"/>
-      <c r="O7" s="161"/>
-      <c r="P7" s="161"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
       <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.3">
@@ -2103,25 +2100,25 @@
     </row>
     <row r="9" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
-      <c r="B9" s="159" t="s">
+      <c r="B9" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="159"/>
-      <c r="D9" s="159"/>
-      <c r="E9" s="160"/>
-      <c r="F9" s="160"/>
-      <c r="G9" s="160"/>
-      <c r="H9" s="160"/>
-      <c r="I9" s="160"/>
-      <c r="J9" s="159" t="s">
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="159"/>
-      <c r="L9" s="161"/>
-      <c r="M9" s="161"/>
-      <c r="N9" s="161"/>
-      <c r="O9" s="161"/>
-      <c r="P9" s="161"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
       <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="1:18" ht="1.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2155,70 +2152,70 @@
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="162"/>
-      <c r="M11" s="162"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="84"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="163"/>
-      <c r="Q11" s="164"/>
+      <c r="P11" s="85"/>
+      <c r="Q11" s="86"/>
     </row>
     <row r="12" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="146"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="146"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="146"/>
-      <c r="M12" s="146"/>
-      <c r="N12" s="146"/>
-      <c r="O12" s="146"/>
-      <c r="P12" s="146"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
       <c r="Q12" s="23"/>
     </row>
     <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="147"/>
-      <c r="C13" s="147"/>
-      <c r="D13" s="147"/>
-      <c r="E13" s="147"/>
-      <c r="F13" s="147"/>
-      <c r="G13" s="147"/>
-      <c r="H13" s="147"/>
-      <c r="I13" s="147"/>
-      <c r="J13" s="147"/>
-      <c r="K13" s="147"/>
-      <c r="L13" s="147"/>
-      <c r="M13" s="147"/>
-      <c r="N13" s="147"/>
-      <c r="O13" s="147"/>
-      <c r="P13" s="147"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
       <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:18" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="148"/>
-      <c r="C14" s="148"/>
-      <c r="D14" s="148"/>
-      <c r="E14" s="148"/>
-      <c r="F14" s="148"/>
-      <c r="G14" s="148"/>
-      <c r="H14" s="148"/>
-      <c r="I14" s="148"/>
-      <c r="J14" s="148"/>
-      <c r="K14" s="148"/>
-      <c r="L14" s="148"/>
-      <c r="M14" s="148"/>
-      <c r="N14" s="148"/>
-      <c r="O14" s="148"/>
-      <c r="P14" s="148"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2245,67 +2242,67 @@
     </row>
     <row r="16" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="149" t="s">
+      <c r="B16" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="149"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="150"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="150"/>
-      <c r="H16" s="149" t="s">
+      <c r="C16" s="91"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="149"/>
-      <c r="J16" s="149"/>
-      <c r="K16" s="149"/>
-      <c r="L16" s="151"/>
-      <c r="M16" s="151"/>
-      <c r="N16" s="151"/>
-      <c r="O16" s="151"/>
-      <c r="P16" s="151"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
       <c r="Q16" s="30"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="152" t="s">
+      <c r="B17" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="152"/>
-      <c r="D17" s="153"/>
-      <c r="E17" s="153"/>
-      <c r="F17" s="153"/>
-      <c r="G17" s="153"/>
-      <c r="H17" s="153"/>
-      <c r="I17" s="153"/>
-      <c r="J17" s="153"/>
-      <c r="K17" s="153"/>
-      <c r="L17" s="155" t="s">
+      <c r="C17" s="94"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="156"/>
-      <c r="N17" s="156"/>
-      <c r="O17" s="156"/>
-      <c r="P17" s="156"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="98"/>
+      <c r="P17" s="98"/>
       <c r="Q17" s="32"/>
     </row>
     <row r="18" spans="1:18" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="152"/>
-      <c r="C18" s="152"/>
-      <c r="D18" s="154"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="154"/>
-      <c r="G18" s="154"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="154"/>
-      <c r="J18" s="154"/>
-      <c r="K18" s="154"/>
-      <c r="L18" s="157"/>
-      <c r="M18" s="158"/>
-      <c r="N18" s="158"/>
-      <c r="O18" s="158"/>
-      <c r="P18" s="158"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="96"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="96"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="100"/>
+      <c r="O18" s="100"/>
+      <c r="P18" s="100"/>
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:18" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2348,159 +2345,159 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
-      <c r="B21" s="137" t="s">
+      <c r="B21" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="137"/>
-      <c r="H21" s="137"/>
-      <c r="I21" s="137"/>
-      <c r="J21" s="137"/>
-      <c r="K21" s="137"/>
-      <c r="L21" s="137"/>
-      <c r="M21" s="137"/>
-      <c r="N21" s="137"/>
-      <c r="O21" s="137"/>
-      <c r="P21" s="137"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="87"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="87"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="87"/>
       <c r="Q21" s="27"/>
       <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="138" t="s">
+      <c r="A22" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="139"/>
-      <c r="C22" s="139"/>
-      <c r="D22" s="139"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="139"/>
-      <c r="G22" s="139"/>
-      <c r="H22" s="139"/>
-      <c r="I22" s="139"/>
-      <c r="J22" s="139"/>
-      <c r="K22" s="139"/>
-      <c r="L22" s="139"/>
-      <c r="M22" s="139"/>
-      <c r="N22" s="139"/>
-      <c r="O22" s="139"/>
-      <c r="P22" s="139"/>
-      <c r="Q22" s="140"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="102"/>
+      <c r="P22" s="102"/>
+      <c r="Q22" s="103"/>
     </row>
     <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
-      <c r="J23" s="144"/>
-      <c r="K23" s="144"/>
-      <c r="L23" s="144"/>
-      <c r="M23" s="144"/>
-      <c r="N23" s="144"/>
-      <c r="O23" s="144"/>
-      <c r="P23" s="144"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="107"/>
+      <c r="J23" s="107"/>
+      <c r="K23" s="107"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="107"/>
+      <c r="O23" s="107"/>
+      <c r="P23" s="107"/>
       <c r="Q23" s="16"/>
     </row>
     <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="144"/>
-      <c r="C24" s="144"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="144"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="144"/>
-      <c r="J24" s="144"/>
-      <c r="K24" s="144"/>
-      <c r="L24" s="144"/>
-      <c r="M24" s="144"/>
-      <c r="N24" s="144"/>
-      <c r="O24" s="144"/>
-      <c r="P24" s="144"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="107"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="107"/>
+      <c r="J24" s="107"/>
+      <c r="K24" s="107"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="107"/>
+      <c r="N24" s="107"/>
+      <c r="O24" s="107"/>
+      <c r="P24" s="107"/>
       <c r="Q24" s="16"/>
     </row>
     <row r="25" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="144"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="144"/>
-      <c r="J25" s="144"/>
-      <c r="K25" s="144"/>
-      <c r="L25" s="144"/>
-      <c r="M25" s="144"/>
-      <c r="N25" s="144"/>
-      <c r="O25" s="144"/>
-      <c r="P25" s="144"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="107"/>
+      <c r="J25" s="107"/>
+      <c r="K25" s="107"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="107"/>
+      <c r="O25" s="107"/>
+      <c r="P25" s="107"/>
       <c r="Q25" s="16"/>
     </row>
     <row r="26" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
-      <c r="B26" s="144"/>
-      <c r="C26" s="144"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="144"/>
-      <c r="H26" s="144"/>
-      <c r="I26" s="144"/>
-      <c r="J26" s="144"/>
-      <c r="K26" s="144"/>
-      <c r="L26" s="144"/>
-      <c r="M26" s="144"/>
-      <c r="N26" s="144"/>
-      <c r="O26" s="144"/>
-      <c r="P26" s="144"/>
+      <c r="B26" s="107"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="107"/>
+      <c r="J26" s="107"/>
+      <c r="K26" s="107"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="107"/>
+      <c r="N26" s="107"/>
+      <c r="O26" s="107"/>
+      <c r="P26" s="107"/>
       <c r="Q26" s="16"/>
     </row>
     <row r="27" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
-      <c r="B27" s="144"/>
-      <c r="C27" s="144"/>
-      <c r="D27" s="144"/>
-      <c r="E27" s="144"/>
-      <c r="F27" s="144"/>
-      <c r="G27" s="144"/>
-      <c r="H27" s="144"/>
-      <c r="I27" s="144"/>
-      <c r="J27" s="144"/>
-      <c r="K27" s="144"/>
-      <c r="L27" s="144"/>
-      <c r="M27" s="144"/>
-      <c r="N27" s="144"/>
-      <c r="O27" s="144"/>
-      <c r="P27" s="144"/>
+      <c r="B27" s="107"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="107"/>
+      <c r="L27" s="107"/>
+      <c r="M27" s="107"/>
+      <c r="N27" s="107"/>
+      <c r="O27" s="107"/>
+      <c r="P27" s="107"/>
       <c r="Q27" s="16"/>
     </row>
     <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="145"/>
-      <c r="I28" s="145"/>
-      <c r="J28" s="145"/>
-      <c r="K28" s="145"/>
-      <c r="L28" s="145"/>
-      <c r="M28" s="145"/>
-      <c r="N28" s="145"/>
-      <c r="O28" s="145"/>
-      <c r="P28" s="145"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="108"/>
+      <c r="H28" s="108"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="108"/>
+      <c r="L28" s="108"/>
+      <c r="M28" s="108"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="108"/>
       <c r="Q28" s="16"/>
     </row>
     <row r="29" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
@@ -2524,401 +2521,401 @@
     </row>
     <row r="30" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
-      <c r="B30" s="141" t="s">
+      <c r="B30" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="141"/>
-      <c r="D30" s="141"/>
+      <c r="C30" s="104"/>
+      <c r="D30" s="104"/>
       <c r="E30" s="43"/>
-      <c r="F30" s="141" t="s">
+      <c r="F30" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="142"/>
-      <c r="H30" s="143" t="s">
+      <c r="G30" s="105"/>
+      <c r="H30" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="141"/>
-      <c r="J30" s="141"/>
-      <c r="K30" s="141"/>
-      <c r="L30" s="141"/>
-      <c r="M30" s="141"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="104"/>
+      <c r="L30" s="104"/>
+      <c r="M30" s="104"/>
       <c r="N30" s="44"/>
-      <c r="O30" s="141" t="s">
+      <c r="O30" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="P30" s="141"/>
+      <c r="P30" s="104"/>
       <c r="Q30" s="45"/>
     </row>
     <row r="31" spans="1:18" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46"/>
-      <c r="B32" s="137" t="s">
+      <c r="B32" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="137"/>
-      <c r="D32" s="137"/>
-      <c r="E32" s="137"/>
-      <c r="F32" s="137"/>
-      <c r="G32" s="137"/>
-      <c r="H32" s="137"/>
-      <c r="I32" s="137"/>
-      <c r="J32" s="137"/>
-      <c r="K32" s="137"/>
-      <c r="L32" s="137"/>
-      <c r="M32" s="137"/>
-      <c r="N32" s="137"/>
-      <c r="O32" s="137"/>
-      <c r="P32" s="137"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="87"/>
+      <c r="N32" s="87"/>
+      <c r="O32" s="87"/>
+      <c r="P32" s="87"/>
       <c r="Q32" s="47"/>
     </row>
     <row r="33" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48"/>
-      <c r="B33" s="132" t="s">
+      <c r="B33" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="132"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="132"/>
-      <c r="F33" s="132"/>
-      <c r="G33" s="132"/>
-      <c r="H33" s="132"/>
-      <c r="I33" s="132"/>
-      <c r="J33" s="132"/>
-      <c r="K33" s="132"/>
-      <c r="L33" s="133"/>
-      <c r="M33" s="134"/>
-      <c r="N33" s="135"/>
-      <c r="O33" s="135"/>
-      <c r="P33" s="135"/>
+      <c r="C33" s="109"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="109"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="109"/>
+      <c r="J33" s="109"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="110"/>
+      <c r="M33" s="111"/>
+      <c r="N33" s="112"/>
+      <c r="O33" s="112"/>
+      <c r="P33" s="112"/>
       <c r="Q33" s="49"/>
     </row>
     <row r="34" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
-      <c r="B34" s="130" t="s">
+      <c r="B34" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="130"/>
-      <c r="D34" s="130"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="130"/>
-      <c r="G34" s="130"/>
-      <c r="H34" s="130"/>
-      <c r="I34" s="130"/>
-      <c r="J34" s="130"/>
-      <c r="K34" s="130"/>
-      <c r="L34" s="131"/>
-      <c r="M34" s="128"/>
-      <c r="N34" s="129"/>
-      <c r="O34" s="129"/>
-      <c r="P34" s="129"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="113"/>
+      <c r="I34" s="113"/>
+      <c r="J34" s="113"/>
+      <c r="K34" s="113"/>
+      <c r="L34" s="114"/>
+      <c r="M34" s="115"/>
+      <c r="N34" s="116"/>
+      <c r="O34" s="116"/>
+      <c r="P34" s="116"/>
       <c r="Q34" s="51"/>
     </row>
     <row r="35" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
-      <c r="B35" s="136" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="136"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="136"/>
+      <c r="B35" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="117"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
       <c r="F35" s="71"/>
-      <c r="G35" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="H35" s="130"/>
-      <c r="I35" s="130"/>
-      <c r="J35" s="130"/>
-      <c r="K35" s="130"/>
-      <c r="L35" s="131"/>
-      <c r="M35" s="128"/>
-      <c r="N35" s="129"/>
-      <c r="O35" s="129"/>
-      <c r="P35" s="129"/>
+      <c r="G35" s="113" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="113"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="113"/>
+      <c r="K35" s="113"/>
+      <c r="L35" s="114"/>
+      <c r="M35" s="115"/>
+      <c r="N35" s="116"/>
+      <c r="O35" s="116"/>
+      <c r="P35" s="116"/>
       <c r="Q35" s="51"/>
     </row>
     <row r="36" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
-      <c r="B36" s="130" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="130"/>
-      <c r="D36" s="130"/>
-      <c r="E36" s="130"/>
+      <c r="B36" s="113" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="113"/>
+      <c r="D36" s="113"/>
+      <c r="E36" s="113"/>
       <c r="F36" s="71"/>
-      <c r="G36" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="H36" s="130"/>
-      <c r="I36" s="130"/>
-      <c r="J36" s="130"/>
-      <c r="K36" s="130"/>
-      <c r="L36" s="131"/>
-      <c r="M36" s="128"/>
-      <c r="N36" s="129"/>
-      <c r="O36" s="129"/>
-      <c r="P36" s="129"/>
+      <c r="G36" s="113" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="113"/>
+      <c r="I36" s="113"/>
+      <c r="J36" s="113"/>
+      <c r="K36" s="113"/>
+      <c r="L36" s="114"/>
+      <c r="M36" s="115"/>
+      <c r="N36" s="116"/>
+      <c r="O36" s="116"/>
+      <c r="P36" s="116"/>
       <c r="Q36" s="51"/>
     </row>
     <row r="37" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
-      <c r="B37" s="130" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="130"/>
-      <c r="D37" s="130"/>
-      <c r="E37" s="130"/>
+      <c r="B37" s="113" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="113"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
       <c r="F37" s="71"/>
-      <c r="G37" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37" s="130"/>
-      <c r="I37" s="130"/>
-      <c r="J37" s="130"/>
-      <c r="K37" s="130"/>
-      <c r="L37" s="131"/>
-      <c r="M37" s="128"/>
-      <c r="N37" s="129"/>
-      <c r="O37" s="129"/>
-      <c r="P37" s="129"/>
+      <c r="G37" s="113" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" s="113"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="113"/>
+      <c r="L37" s="114"/>
+      <c r="M37" s="115"/>
+      <c r="N37" s="116"/>
+      <c r="O37" s="116"/>
+      <c r="P37" s="116"/>
       <c r="Q37" s="51"/>
     </row>
     <row r="38" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
-      <c r="B38" s="130"/>
-      <c r="C38" s="130"/>
-      <c r="D38" s="130"/>
-      <c r="E38" s="130"/>
-      <c r="F38" s="130"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="130"/>
-      <c r="I38" s="130"/>
-      <c r="J38" s="130"/>
-      <c r="K38" s="130"/>
-      <c r="L38" s="131"/>
-      <c r="M38" s="128"/>
-      <c r="N38" s="129"/>
-      <c r="O38" s="129"/>
-      <c r="P38" s="129"/>
+      <c r="B38" s="113"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="113"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="113"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="114"/>
+      <c r="M38" s="115"/>
+      <c r="N38" s="116"/>
+      <c r="O38" s="116"/>
+      <c r="P38" s="116"/>
       <c r="Q38" s="51"/>
     </row>
     <row r="39" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
-      <c r="B39" s="101" t="s">
+      <c r="B39" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101"/>
-      <c r="G39" s="101"/>
-      <c r="H39" s="101"/>
-      <c r="I39" s="101"/>
-      <c r="J39" s="101"/>
-      <c r="K39" s="101"/>
-      <c r="L39" s="102"/>
-      <c r="M39" s="103"/>
-      <c r="N39" s="104"/>
-      <c r="O39" s="104"/>
-      <c r="P39" s="104"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="118"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="118"/>
+      <c r="H39" s="118"/>
+      <c r="I39" s="118"/>
+      <c r="J39" s="118"/>
+      <c r="K39" s="118"/>
+      <c r="L39" s="119"/>
+      <c r="M39" s="120"/>
+      <c r="N39" s="121"/>
+      <c r="O39" s="121"/>
+      <c r="P39" s="121"/>
       <c r="Q39" s="53"/>
     </row>
     <row r="40" spans="1:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:17" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="54"/>
-      <c r="B41" s="105" t="s">
+      <c r="B41" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="105"/>
-      <c r="D41" s="107" t="s">
+      <c r="C41" s="122"/>
+      <c r="D41" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="108"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="113" t="s">
+      <c r="E41" s="125"/>
+      <c r="F41" s="126"/>
+      <c r="G41" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
-      <c r="J41" s="114"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="117" t="s">
+      <c r="H41" s="131"/>
+      <c r="I41" s="131"/>
+      <c r="J41" s="131"/>
+      <c r="K41" s="131"/>
+      <c r="L41" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="M41" s="118"/>
-      <c r="N41" s="118"/>
-      <c r="O41" s="118"/>
-      <c r="P41" s="118"/>
+      <c r="M41" s="135"/>
+      <c r="N41" s="135"/>
+      <c r="O41" s="135"/>
+      <c r="P41" s="135"/>
       <c r="Q41" s="55"/>
     </row>
     <row r="42" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
-      <c r="B42" s="106"/>
-      <c r="C42" s="106"/>
-      <c r="D42" s="110"/>
-      <c r="E42" s="111"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="115"/>
-      <c r="H42" s="116"/>
-      <c r="I42" s="116"/>
-      <c r="J42" s="116"/>
-      <c r="K42" s="116"/>
-      <c r="L42" s="119"/>
-      <c r="M42" s="120"/>
-      <c r="N42" s="120"/>
-      <c r="O42" s="120"/>
-      <c r="P42" s="120"/>
+      <c r="B42" s="123"/>
+      <c r="C42" s="123"/>
+      <c r="D42" s="127"/>
+      <c r="E42" s="128"/>
+      <c r="F42" s="129"/>
+      <c r="G42" s="132"/>
+      <c r="H42" s="133"/>
+      <c r="I42" s="133"/>
+      <c r="J42" s="133"/>
+      <c r="K42" s="133"/>
+      <c r="L42" s="136"/>
+      <c r="M42" s="137"/>
+      <c r="N42" s="137"/>
+      <c r="O42" s="137"/>
+      <c r="P42" s="137"/>
       <c r="Q42" s="57"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
-      <c r="B43" s="106"/>
-      <c r="C43" s="106"/>
-      <c r="D43" s="110"/>
-      <c r="E43" s="111"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="115"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="116"/>
-      <c r="J43" s="116"/>
-      <c r="K43" s="116"/>
-      <c r="L43" s="119"/>
-      <c r="M43" s="120"/>
-      <c r="N43" s="120"/>
-      <c r="O43" s="120"/>
-      <c r="P43" s="120"/>
+      <c r="B43" s="123"/>
+      <c r="C43" s="123"/>
+      <c r="D43" s="127"/>
+      <c r="E43" s="128"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="132"/>
+      <c r="H43" s="133"/>
+      <c r="I43" s="133"/>
+      <c r="J43" s="133"/>
+      <c r="K43" s="133"/>
+      <c r="L43" s="136"/>
+      <c r="M43" s="137"/>
+      <c r="N43" s="137"/>
+      <c r="O43" s="137"/>
+      <c r="P43" s="137"/>
       <c r="Q43" s="57"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="56"/>
-      <c r="B44" s="106"/>
-      <c r="C44" s="106"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="122"/>
-      <c r="F44" s="123"/>
-      <c r="G44" s="124"/>
-      <c r="H44" s="125"/>
-      <c r="I44" s="125"/>
-      <c r="J44" s="125"/>
-      <c r="K44" s="125"/>
-      <c r="L44" s="126"/>
-      <c r="M44" s="127"/>
-      <c r="N44" s="127"/>
-      <c r="O44" s="127"/>
-      <c r="P44" s="127"/>
+      <c r="B44" s="123"/>
+      <c r="C44" s="123"/>
+      <c r="D44" s="138"/>
+      <c r="E44" s="139"/>
+      <c r="F44" s="140"/>
+      <c r="G44" s="141"/>
+      <c r="H44" s="142"/>
+      <c r="I44" s="142"/>
+      <c r="J44" s="142"/>
+      <c r="K44" s="142"/>
+      <c r="L44" s="143"/>
+      <c r="M44" s="144"/>
+      <c r="N44" s="144"/>
+      <c r="O44" s="144"/>
+      <c r="P44" s="144"/>
       <c r="Q44" s="57"/>
     </row>
     <row r="45" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56"/>
-      <c r="B45" s="106"/>
-      <c r="C45" s="106"/>
-      <c r="D45" s="121"/>
-      <c r="E45" s="122"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="125"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="125"/>
-      <c r="K45" s="125"/>
-      <c r="L45" s="126"/>
-      <c r="M45" s="127"/>
-      <c r="N45" s="127"/>
-      <c r="O45" s="127"/>
-      <c r="P45" s="127"/>
+      <c r="B45" s="123"/>
+      <c r="C45" s="123"/>
+      <c r="D45" s="138"/>
+      <c r="E45" s="139"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="141"/>
+      <c r="H45" s="142"/>
+      <c r="I45" s="142"/>
+      <c r="J45" s="142"/>
+      <c r="K45" s="142"/>
+      <c r="L45" s="143"/>
+      <c r="M45" s="144"/>
+      <c r="N45" s="144"/>
+      <c r="O45" s="144"/>
+      <c r="P45" s="144"/>
       <c r="Q45" s="57"/>
     </row>
     <row r="46" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="58"/>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="145" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="93"/>
-      <c r="G46" s="94"/>
-      <c r="H46" s="95"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="95"/>
-      <c r="K46" s="95"/>
-      <c r="L46" s="96"/>
-      <c r="M46" s="97"/>
-      <c r="N46" s="97"/>
-      <c r="O46" s="97"/>
-      <c r="P46" s="97"/>
+      <c r="C46" s="145"/>
+      <c r="D46" s="146"/>
+      <c r="E46" s="147"/>
+      <c r="F46" s="148"/>
+      <c r="G46" s="149"/>
+      <c r="H46" s="150"/>
+      <c r="I46" s="150"/>
+      <c r="J46" s="150"/>
+      <c r="K46" s="150"/>
+      <c r="L46" s="151"/>
+      <c r="M46" s="152"/>
+      <c r="N46" s="152"/>
+      <c r="O46" s="152"/>
+      <c r="P46" s="152"/>
       <c r="Q46" s="59"/>
     </row>
     <row r="47" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
-      <c r="B47" s="81" t="s">
+      <c r="B47" s="153" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="81"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="83"/>
-      <c r="F47" s="84"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="86"/>
-      <c r="I47" s="86"/>
-      <c r="J47" s="86"/>
-      <c r="K47" s="86"/>
-      <c r="L47" s="99"/>
-      <c r="M47" s="100"/>
-      <c r="N47" s="100"/>
-      <c r="O47" s="100"/>
-      <c r="P47" s="100"/>
+      <c r="C47" s="153"/>
+      <c r="D47" s="154"/>
+      <c r="E47" s="155"/>
+      <c r="F47" s="156"/>
+      <c r="G47" s="157"/>
+      <c r="H47" s="158"/>
+      <c r="I47" s="158"/>
+      <c r="J47" s="158"/>
+      <c r="K47" s="158"/>
+      <c r="L47" s="159"/>
+      <c r="M47" s="160"/>
+      <c r="N47" s="160"/>
+      <c r="O47" s="160"/>
+      <c r="P47" s="160"/>
       <c r="Q47" s="62"/>
     </row>
     <row r="48" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="63"/>
-      <c r="B48" s="73" t="s">
+      <c r="B48" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="73"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="78"/>
-      <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
-      <c r="K48" s="78"/>
-      <c r="L48" s="79"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="80"/>
-      <c r="P48" s="80"/>
+      <c r="C48" s="162"/>
+      <c r="D48" s="163"/>
+      <c r="E48" s="164"/>
+      <c r="F48" s="165"/>
+      <c r="G48" s="166"/>
+      <c r="H48" s="167"/>
+      <c r="I48" s="167"/>
+      <c r="J48" s="167"/>
+      <c r="K48" s="167"/>
+      <c r="L48" s="168"/>
+      <c r="M48" s="169"/>
+      <c r="N48" s="169"/>
+      <c r="O48" s="169"/>
+      <c r="P48" s="169"/>
       <c r="Q48" s="64"/>
     </row>
     <row r="49" spans="1:17" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="61"/>
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="81"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="83"/>
-      <c r="F49" s="84"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="86"/>
-      <c r="I49" s="86"/>
-      <c r="J49" s="86"/>
-      <c r="K49" s="86"/>
-      <c r="L49" s="87"/>
-      <c r="M49" s="88"/>
-      <c r="N49" s="88"/>
-      <c r="O49" s="88"/>
-      <c r="P49" s="88"/>
+      <c r="C49" s="153"/>
+      <c r="D49" s="154"/>
+      <c r="E49" s="155"/>
+      <c r="F49" s="156"/>
+      <c r="G49" s="170"/>
+      <c r="H49" s="158"/>
+      <c r="I49" s="158"/>
+      <c r="J49" s="158"/>
+      <c r="K49" s="158"/>
+      <c r="L49" s="171"/>
+      <c r="M49" s="172"/>
+      <c r="N49" s="172"/>
+      <c r="O49" s="172"/>
+      <c r="P49" s="172"/>
       <c r="Q49" s="62"/>
     </row>
     <row r="50" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="65"/>
-      <c r="B50" s="89" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
+      <c r="B50" s="173" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="173"/>
+      <c r="D50" s="173"/>
+      <c r="E50" s="173"/>
+      <c r="F50" s="173"/>
       <c r="G50" s="66"/>
       <c r="H50" s="66"/>
       <c r="I50" s="66"/>
@@ -2933,42 +2930,74 @@
     </row>
     <row r="51" spans="1:17" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="69"/>
-      <c r="B51" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="72"/>
-      <c r="L51" s="72"/>
-      <c r="M51" s="72"/>
-      <c r="N51" s="72"/>
-      <c r="O51" s="72"/>
-      <c r="P51" s="72"/>
+      <c r="B51" s="161"/>
+      <c r="C51" s="161"/>
+      <c r="D51" s="161"/>
+      <c r="E51" s="161"/>
+      <c r="F51" s="161"/>
+      <c r="G51" s="161"/>
+      <c r="H51" s="161"/>
+      <c r="I51" s="161"/>
+      <c r="J51" s="161"/>
+      <c r="K51" s="161"/>
+      <c r="L51" s="161"/>
+      <c r="M51" s="161"/>
+      <c r="N51" s="161"/>
+      <c r="O51" s="161"/>
+      <c r="P51" s="161"/>
       <c r="Q51" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="D1:Q1"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D3:Q3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B51:P51"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="G48:K48"/>
+    <mergeCell ref="L48:P48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="G49:K49"/>
+    <mergeCell ref="L49:P49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="L46:P46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="L47:P47"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="D41:F43"/>
+    <mergeCell ref="G41:K43"/>
+    <mergeCell ref="L41:P43"/>
+    <mergeCell ref="D44:F45"/>
+    <mergeCell ref="G44:K45"/>
+    <mergeCell ref="L44:P45"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="G36:L36"/>
+    <mergeCell ref="G37:L37"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="G35:L35"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="A22:Q22"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="B23:P28"/>
     <mergeCell ref="B21:P21"/>
     <mergeCell ref="B12:P13"/>
     <mergeCell ref="B14:P14"/>
@@ -2981,55 +3010,21 @@
     <mergeCell ref="L17:P17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="L18:P18"/>
-    <mergeCell ref="B32:P32"/>
-    <mergeCell ref="A22:Q22"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="B23:P28"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="G35:L35"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="M37:P37"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="G36:L36"/>
-    <mergeCell ref="G37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D41:F43"/>
-    <mergeCell ref="G41:K43"/>
-    <mergeCell ref="L41:P43"/>
-    <mergeCell ref="D44:F45"/>
-    <mergeCell ref="G44:K45"/>
-    <mergeCell ref="L44:P45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="L46:P46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="L47:P47"/>
-    <mergeCell ref="B51:P51"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="L48:P48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="G49:K49"/>
-    <mergeCell ref="L49:P49"/>
-    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="D1:Q1"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D3:Q3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
@@ -3047,15 +3042,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D262036FF67A5D43BF6E290DEB360352" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c503d2a7b448377a6cc9e75158e3af5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e744003-367c-4be8-bc40-2385cb622540" xmlns:ns3="0930cf9b-719b-4120-8db4-f84070340397" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9cea96fa3cc1abdf61d90e2bf9fac8d2" ns2:_="" ns3:_="">
     <xsd:import namespace="4e744003-367c-4be8-bc40-2385cb622540"/>
@@ -3272,6 +3258,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
   <ds:schemaRefs>
@@ -3290,14 +3285,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3DC5811-E2D9-4774-B143-A47CE40C3F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3314,4 +3301,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>